<commit_message>
TP11 Actualizado, Casos de Prueba Corregidos
</commit_message>
<xml_diff>
--- a/Practico/TPs/TP11/Resolucion-TP11-Ezequiel.xlsx
+++ b/Practico/TPs/TP11/Resolucion-TP11-Ezequiel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://frcutneduar-my.sharepoint.com/personal/67788_sistemas_frc_utn_edu_ar/Documents/Ingenieria de Software - 4K2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{F05F2A51-D567-437A-8E74-F8FAB535CAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBFF779F-53C9-46EA-8F96-ED568DBAEB98}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{F05F2A51-D567-437A-8E74-F8FAB535CAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF1BB69B-8515-4F53-BB29-EBB52D300EEA}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-2175" windowWidth="24240" windowHeight="13140" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-2175" windowWidth="24240" windowHeight="13140" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla de Test - Caja Negra" sheetId="29" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="140">
   <si>
     <t>TC_001</t>
   </si>
@@ -344,23 +344,11 @@
     <t>Direccion de Comercio</t>
   </si>
   <si>
-    <t>*No ingresa direccion de comercio
-*No ingresa calle del comercio
-*No ingresa numero de calle</t>
-  </si>
-  <si>
     <t>*ingresar 0 como numero de calle
 *ingresar 1 como numero de calle</t>
   </si>
   <si>
     <t>Direccion de la Entrega</t>
-  </si>
-  <si>
-    <t>*No ingresa direccion de la entrega
-*No ingresa calle de la entrega
-*No ingresa numero de calle
-*Ingresa numero de calle con letras o mayor de 4 cifras
-*ingresa calle de la entrega invalida</t>
   </si>
   <si>
     <t>*ingresar 0 como numero de calle
@@ -449,79 +437,10 @@
     <t>Probar Realizar Pedido de “lo que sea” ingresando Especificacion,  ingresando Ciudad, Direccion de Comercio y de Entrega, seleccionando Tarjeta de Credito/Debito como Forma de Pago y seleccionando "Lo antes Posible" para la Entrega, usando una TARJETA VISA</t>
   </si>
   <si>
-    <t>1- el comprador selecciona "Realizar Pedido de lo que sea"
-2- el sistema solicita el ingreso de la especifiacion del producto y la imagen
-3- el comprador ingresa en el campo de texto la especifiacion del producto: "Gorra Adidas Negra"
-4- el comprador no sube la imagen del producto
-5- El sistema confirma que se ingreso una especificacion y si hay alguna imagen cargada, pasa 
-6- El sisema pide la direccion del comercio
-7- El comprador selecciona la ciudad del comercio: "Cordoba"
-8- El comprador ingresa en el campo de texto la direccion del comercio sin referencia: "Juan B Justo 1234"
-9- el sistema verifica que se haya elegido alguna ciudad e ingresado alguna direccion del comercio, pasa
-10- El sistema solicita la direccion de entrega
-11- el comprador selecciona la ciudad de la direccion de la entrega: "Cordoba"
-12- El sistema verifica que sea la misma ciudad que de la direccion del comercio, pasa
-13-  El comprador ingresa la direccion de entrega con alguna referencia: "Mariano Fragueiro 1122", "Casa blanca de Rejas Verdes"
-14- el sistema verifica si es valida las direccion de entrega, pasa
-15- el sistema solicita la seleccion de la forma de pago
-16- el comprador selecciona "Tarjeta de Credito/Debito" como forma de pago
-17- el sistema solicita los datos de la Tarjeta
-18- el comprador ingresa "4111 2222 3333 4444", "Quiroga Jorge", "10/2022", "111"
-19- el sistema verifica los datos de la tarjeta, y confirma
-20- el sistema solicita la fecha y hora de entrega
-21- el compador selecciona "Lo antes Posible"
-22- el sistema verifica que se haya ingresado alguna fecha de recepcion o "lo antes posible", y confirma
-23- el sistema solicita la finalizacion del pedido
-24- el comprador confirma la finalizacion del pedido</t>
-  </si>
-  <si>
-    <t>finalizar Pedido de lo que sea con tarejta visa exitosamente</t>
-  </si>
-  <si>
-    <t>finalizar Pedido de lo que sea con tarejta MasterCard exitosamente</t>
-  </si>
-  <si>
     <t>Probar Realizar Pedido de “lo que sea” ingresando Especificacion,  ingresando Ciudad, Direccion de Comercio y de Entrega, seleccionando Tarjeta de Credito/Debito como Forma de Pago y seleccionando "Lo antes Posible" para la Entrega, usando una TARJETA MASTERCARD</t>
   </si>
   <si>
-    <t>1- el comprador selecciona "Realizar Pedido de lo que sea"
-2- el sistema solicita el ingreso de la especifiacion del producto y la imagen
-3- el comprador ingresa en el campo de texto la especifiacion del producto: "Gorra Adidas Negra"
-4- el comprador no sube la imagen del producto
-5- El sistema confirma que se ingreso una especificacion y si hay alguna imagen cargada, pasa 
-6- El sisema pide la direccion del comercio
-7- El comprador selecciona la ciudad del comercio: "Cordoba"
-8- El comprador ingresa en el campo de texto la direccion del comercio sin referencia: "Juan B Justo 1234"
-9- el sistema verifica que se haya elegido alguna ciudad e ingresado alguna direccion del comercio, pasa
-10- El sistema solicita la direccion de entrega
-11- el comprador selecciona la ciudad de la direccion de la entrega: "Cordoba"
-12- El sistema verifica que sea la misma ciudad que de la direccion del comercio, pasa
-13-  El comprador ingresa la direccion de entrega con alguna referencia: "Mariano Fragueiro 1122", "Casa blanca de Rejas Verdes"
-14- el sistema verifica si es valida las direccion de entrega, pasa
-15- el sistema solicita la seleccion de la forma de pago
-16- el comprador selecciona "Tarjeta de Credito/Debito" como forma de pago
-17- el sistema solicita los datos de la Tarjeta
-18- el comprador ingresa "5111 2222 3333 4444", "Quiroga Jorge", "08/2024", "111"
-19- el sistema verifica los datos de la tarjeta, y confirma
-20- el sistema solicita la fecha y hora de entrega
-21- el compador selecciona "Lo antes Posible"
-22- el sistema verifica que se haya ingresado alguna fecha de recepcion o "lo antes posible", y confirma
-23- el sistema solicita la finalizacion del pedido
-24- el comprador confirma la finalizacion del pedido</t>
-  </si>
-  <si>
     <t>*seleccionar una Ciudad de las disponibles y que la ciudad del comercio es la misma de la Direccion de Entrega</t>
-  </si>
-  <si>
-    <t>*Ingresa Direccion de Comercio con calle, numero 
-*Ingresa referencia de la Direccion
-*No ingresa referencia de direccion del comercio</t>
-  </si>
-  <si>
-    <t>*Ingresa Direccion de la Entrega con calle, numero 
-*Ingresa referencia de la Direccion
-*No ingresa referencia de direccion de la Entrega
-*Ingresa Numero de calle con solo numeros y hasta 4 cifras</t>
   </si>
   <si>
     <t>*Ingresa Monto a pagar solo numeros
@@ -533,12 +452,6 @@
 *Ingresa fecha de Vencimiento de Tarjeta y con formato (MM/AAAA)
 *Ingresa CVC de la Tarjeta con 3 cifras y numeros 
 *Fecha de vencimiento mayor o igual al mes actual</t>
-  </si>
-  <si>
-    <t>el Comprador debe estar logueado en la app
-fecha actual= 25/10/2022 13:30
-Ciudad Villa Carlos Paz esta cargada en la app
-precio de envio: $300 por metro lineal + un costo base de $500</t>
   </si>
   <si>
     <t>1- el comprador selecciona "Realizar Pedido de lo que sea"
@@ -554,12 +467,76 @@
 11- el comprador confirma la finalizacion del pedido</t>
   </si>
   <si>
+    <t>RELEVANTE PARA HACER CASOS DE PRUEBA</t>
+  </si>
+  <si>
+    <t>fecha actual= 25/10/2022 13:30
+Ciudad Villa Carlos Paz esta cargada en la app
+precio de envio: $300 por metro lineal + un costo base de $500</t>
+  </si>
+  <si>
+    <t>fecha actual= 25/10/2022 13:30
+Cordoba esta cargada en la app
+precio de envio: $300 por metro lineal + un costo base de $500</t>
+  </si>
+  <si>
+    <t>1- el comprador selecciona "Realizar Pedido de lo que sea"
+2- el comprador ingresa en el campo de texto la especifiacion del producto: "Gorra Adidas Negra"
+3- el comprador no sube la imagen del producto
+4- El comprador selecciona la ciudad del comercio: "Cordoba"
+5- El comprador ingresa en el campo de texto la direccion del comercio sin referencia: "Juan B Justo 1234"
+6- el comprador selecciona la ciudad de la direccion de la entrega: "Cordoba"
+7-  El comprador ingresa la direccion de entrega con alguna referencia: "Mariano Fragueiro 1122", "Casa blanca de Rejas Verdes"
+8- el comprador selecciona "Tarjeta de Credito/Debito" como forma de pago
+9- el comprador ingresa "4111 2222 3333 4444", "Quiroga Jorge", "10/2022", "111"
+10- el compador selecciona "Lo antes Posible"
+11- el comprador confirma la finalizacion del pedido</t>
+  </si>
+  <si>
     <t>1- el sistema muestra el ingreso de especificacion del producto y el ingreso de imagen
-8- el sistema solicita el ingreso del monto a abonar y el valor del pago total : "3000"
+8- el sistema solicita los datos de la Tarjeta y muestra el monto total
 11- el sistema muestra un mensaje de que  el pedido se realizo exitosamente</t>
   </si>
   <si>
-    <t>RELEVANTE PARA HACER CASOS DE PRUEBA</t>
+    <t>1- el sistema muestra el ingreso de especificacion del producto y el ingreso de imagen
+8- el sistema solicita el ingreso del monto a abonar y el valor del pago total
+11- el sistema muestra un mensaje de que  el pedido se realizo exitosamente</t>
+  </si>
+  <si>
+    <t>1- el comprador selecciona "Realizar Pedido de lo que sea"
+2- el comprador ingresa en el campo de texto la especifiacion del producto: "Gorra Adidas Negra"
+3- el comprador no sube la imagen del producto
+4- El comprador selecciona la ciudad del comercio: "Cordoba"
+5- El comprador ingresa en el campo de texto la direccion del comercio sin referencia: "Juan B Justo 1234"
+6- el comprador selecciona la ciudad de la direccion de la entrega: "Cordoba"
+7-  El comprador ingresa la direccion de entrega con alguna referencia: "Mariano Fragueiro 1122", "Casa blanca de Rejas Verdes"
+8- el comprador selecciona "Tarjeta de Credito/Debito" como forma de pago
+9- el comprador ingresa "5111 2222 3333 4444", "Quiroga Jorge", "12/2022", "222"
+10- el compador selecciona "Lo antes Posible"
+11- el comprador confirma la finalizacion del pedido</t>
+  </si>
+  <si>
+    <t>*Ingresa calle de comercio 
+*Ingresa numero de calle de Comercio y solo numero y hasta 4 cifras
+*Ingresa referencia de la Direccion
+*No ingresa referencia de direccion del comercio</t>
+  </si>
+  <si>
+    <t>*Ingresa calle de Entrega
+*Ingresa numero de calle de Entrega y solo numeros y hasta 4 cifras
+*No ingresa referencia de direccion de la Entrega</t>
+  </si>
+  <si>
+    <t>*No ingresa direccion de comercio
+*No ingresa calle del comercio
+*No ingresa numero de calle
+*Ingresa numero de calle con letras o mayor de 4 cifras</t>
+  </si>
+  <si>
+    <t>*No ingresa direccion de la entrega
+*No ingresa calle de la entrega
+*No ingresa numero de calle
+*Ingresa numero de calle con letras o mayor de 4 cifras</t>
   </si>
 </sst>
 </file>
@@ -1385,6 +1362,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1411,18 +1400,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2235,76 +2212,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9AF0F5-701D-4995-8BE8-1AD93624257C}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17:N19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="3" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="63" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="66" t="s">
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="68" t="s">
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="M4" s="69"/>
-      <c r="N4" s="70"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="74"/>
     </row>
     <row r="5" spans="1:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54">
         <v>1</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="73" t="s">
+      <c r="C5" s="63"/>
+      <c r="D5" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73" t="s">
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73" t="s">
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
     </row>
     <row r="6" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="55"/>
@@ -2380,7 +2357,7 @@
       <c r="M9" s="61"/>
       <c r="N9" s="61"/>
       <c r="O9" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -2408,7 +2385,7 @@
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="60" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E11" s="60"/>
       <c r="F11" s="60"/>
@@ -2464,19 +2441,19 @@
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="60" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
       <c r="G14" s="60"/>
       <c r="H14" s="60" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="I14" s="60"/>
       <c r="J14" s="60"/>
       <c r="K14" s="60"/>
       <c r="L14" s="60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M14" s="61"/>
       <c r="N14" s="61"/>
@@ -2497,7 +2474,7 @@
       <c r="M15" s="61"/>
       <c r="N15" s="61"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="57"/>
       <c r="B16" s="58"/>
       <c r="C16" s="59"/>
@@ -2518,23 +2495,23 @@
         <v>5</v>
       </c>
       <c r="B17" s="59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="60" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E17" s="60"/>
       <c r="F17" s="60"/>
       <c r="G17" s="60"/>
       <c r="H17" s="60" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="I17" s="60"/>
       <c r="J17" s="60"/>
       <c r="K17" s="60"/>
       <c r="L17" s="60" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M17" s="61"/>
       <c r="N17" s="61"/>
@@ -2555,7 +2532,7 @@
       <c r="M18" s="61"/>
       <c r="N18" s="61"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="53"/>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
@@ -2576,17 +2553,17 @@
         <v>6</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C20" s="59"/>
       <c r="D20" s="60" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E20" s="60"/>
       <c r="F20" s="60"/>
       <c r="G20" s="60"/>
       <c r="H20" s="60" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I20" s="60"/>
       <c r="J20" s="60"/>
@@ -2632,23 +2609,23 @@
         <v>7</v>
       </c>
       <c r="B23" s="59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C23" s="59"/>
       <c r="D23" s="60" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E23" s="60"/>
       <c r="F23" s="60"/>
       <c r="G23" s="60"/>
       <c r="H23" s="60" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I23" s="60"/>
       <c r="J23" s="60"/>
       <c r="K23" s="60"/>
       <c r="L23" s="60" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M23" s="61"/>
       <c r="N23" s="61"/>
@@ -2669,7 +2646,7 @@
       <c r="M24" s="61"/>
       <c r="N24" s="61"/>
       <c r="O24" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -2693,23 +2670,23 @@
         <v>8</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C26" s="59"/>
       <c r="D26" s="60" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E26" s="60"/>
       <c r="F26" s="60"/>
       <c r="G26" s="60"/>
       <c r="H26" s="60" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I26" s="60"/>
       <c r="J26" s="60"/>
       <c r="K26" s="60"/>
       <c r="L26" s="60" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M26" s="61"/>
       <c r="N26" s="61"/>
@@ -2746,7 +2723,7 @@
       <c r="M28" s="61"/>
       <c r="N28" s="61"/>
       <c r="O28" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2754,23 +2731,23 @@
         <v>9</v>
       </c>
       <c r="B29" s="59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C29" s="59"/>
       <c r="D29" s="60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E29" s="60"/>
       <c r="F29" s="60"/>
       <c r="G29" s="60"/>
       <c r="H29" s="60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I29" s="60"/>
       <c r="J29" s="60"/>
       <c r="K29" s="60"/>
       <c r="L29" s="60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M29" s="61"/>
       <c r="N29" s="61"/>
@@ -2807,7 +2784,7 @@
       <c r="M31" s="61"/>
       <c r="N31" s="61"/>
       <c r="O31" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -2878,9 +2855,9 @@
   </sheetPr>
   <dimension ref="A1:AS73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3050,7 +3027,7 @@
       <c r="B5" s="77"/>
       <c r="C5" s="43"/>
       <c r="D5" s="79" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E5" s="80"/>
       <c r="F5" s="81"/>
@@ -3237,22 +3214,22 @@
         <v>0</v>
       </c>
       <c r="B11" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>122</v>
-      </c>
       <c r="E11" s="26" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="15"/>
@@ -3276,27 +3253,27 @@
       <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
     </row>
-    <row r="12" spans="1:45" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="300" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="15"/>
@@ -3320,27 +3297,27 @@
       <c r="AR12" s="7"/>
       <c r="AS12" s="7"/>
     </row>
-    <row r="13" spans="1:45" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="300" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C13" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="D13" s="26" t="s">
-        <v>129</v>
-      </c>
       <c r="E13" s="26" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="15"/>
@@ -3364,7 +3341,7 @@
       <c r="AR13" s="7"/>
       <c r="AS13" s="7"/>
     </row>
-    <row r="14" spans="1:45" ht="324" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>42</v>
       </c>
@@ -3372,9 +3349,7 @@
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="26"/>
-      <c r="F14" s="26" t="s">
-        <v>137</v>
-      </c>
+      <c r="F14" s="26"/>
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
       <c r="I14" s="15"/>

</xml_diff>

<commit_message>
TP11 - Campo Direccion Corregido
</commit_message>
<xml_diff>
--- a/Practico/TPs/TP11/Resolucion-TP11-Ezequiel.xlsx
+++ b/Practico/TPs/TP11/Resolucion-TP11-Ezequiel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\Documents\GitHub\ISW-Grupo2-4K2-2022\Practico\TPs\TP11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E66A762-849A-4189-9837-F80BBA1AAB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{839C8E9F-B7BB-4178-B290-8B63A9B7C862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="159">
   <si>
     <t>TC_001</t>
   </si>
@@ -339,34 +339,6 @@
   <si>
     <t>*No selecciona ninguna Ciudad
 *La ciudad del comercio no es la misma que de la Direccion de Entrega</t>
-  </si>
-  <si>
-    <t>Direccion de Comercio</t>
-  </si>
-  <si>
-    <t>*No ingresa direccion de comercio
-*No ingresa calle del comercio
-*No ingresa numero de calle</t>
-  </si>
-  <si>
-    <t>*ingresar 0 como numero de calle
-*ingresar 1 como numero de calle</t>
-  </si>
-  <si>
-    <t>Direccion de la Entrega</t>
-  </si>
-  <si>
-    <t>*No ingresa direccion de la entrega
-*No ingresa calle de la entrega
-*No ingresa numero de calle
-*Ingresa numero de calle con letras o mayor de 4 cifras
-*ingresa calle de la entrega invalida</t>
-  </si>
-  <si>
-    <t>*ingresar 0 como numero de calle
-*ingresar 1 como numero de calle
-*ingresar 1234 como numero de calle
-*ingresar 12345 como numero de calle</t>
   </si>
   <si>
     <t>Forma de Pago</t>
@@ -491,17 +463,6 @@
     <t>*seleccionar una Ciudad de las disponibles y que la ciudad del comercio es la misma de la Direccion de Entrega</t>
   </si>
   <si>
-    <t>*Ingresa Direccion de Comercio con calle, numero 
-*Ingresa referencia de la Direccion
-*No ingresa referencia de direccion del comercio</t>
-  </si>
-  <si>
-    <t>*Ingresa Direccion de la Entrega con calle, numero 
-*Ingresa referencia de la Direccion
-*No ingresa referencia de direccion de la Entrega
-*Ingresa Numero de calle con solo numeros y hasta 4 cifras</t>
-  </si>
-  <si>
     <t>*Ingresa Monto a pagar solo numeros
 *Ingresa monto mayor o igual al total a pagar</t>
   </si>
@@ -530,9 +491,6 @@
 11- el sistema muestra un mensaje de que  el pedido se realizo exitosamente</t>
   </si>
   <si>
-    <t>RELEVANTE PARA HACER CASOS DE PRUEBA</t>
-  </si>
-  <si>
     <t>Nro Tajeta de Credito/Debito</t>
   </si>
   <si>
@@ -591,6 +549,71 @@
   <si>
     <t>*No selecciona fecha de vencimiento
 *Selecciona una fecha de vencimiento anterior a la actual</t>
+  </si>
+  <si>
+    <t>Calle Direccion Comercio</t>
+  </si>
+  <si>
+    <t>* Ingresa calle de direccion de comercio, con calle que pertenezca a la Ciudad seleccionada</t>
+  </si>
+  <si>
+    <t>* No ingresa calle de direccion de comercio
+* Ingresa calle de direccion de comercio, con calle que no pertenezca a la ciudad seleccionada</t>
+  </si>
+  <si>
+    <t>* Ingrersa numero para altura de direccion de comercio, mayor a 0 y menos a 10000</t>
+  </si>
+  <si>
+    <t>Altura Direccion Comercio</t>
+  </si>
+  <si>
+    <t>* No ingresa altura de direccion de comercio
+* Ingresa altura con valores no numericos
+* Ingresa altura con valor &lt;= 0
+* Ingresa altura con valor &gt;= 10000</t>
+  </si>
+  <si>
+    <t>Referencia Direccion Entrega</t>
+  </si>
+  <si>
+    <t>Calle Direccion Entrega</t>
+  </si>
+  <si>
+    <t>* Ingresa calle de direccion de entrega, con calle que pertenezca a la Ciudad seleccionada</t>
+  </si>
+  <si>
+    <t>* No ingresa calle de direccion de entrega
+* Ingresa calle de direccion de entrega, con calle que no pertenezca a la ciudad seleccionada</t>
+  </si>
+  <si>
+    <t>Altura Direccion Entrega</t>
+  </si>
+  <si>
+    <t>* Ingrersa numero para altura de direccion de entrega, mayor a 0 y menos a 10000</t>
+  </si>
+  <si>
+    <t>* No ingresa altura de direccion de entrega
+* Ingresa altura con valores no numericos
+* Ingresa altura con valor &lt;= 0
+* Ingresa altura con valor &gt;= 10000</t>
+  </si>
+  <si>
+    <t>Referencia Direccion Comercio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Ingresa 0 como altura
+* Ingresa 1 como altura
+* Ingresa 9999 como altura
+* Ingresa 10000 como altura
+</t>
+  </si>
+  <si>
+    <t>* Ingresa referencia para la direccion de comercio 
+* No ingresa referencia para la direccion de comercio</t>
+  </si>
+  <si>
+    <t>* Ingresa referencia para la direccion de entrega
+* No ingresa referencia para la direccion de entrega</t>
   </si>
 </sst>
 </file>
@@ -787,7 +810,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1244,6 +1267,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1261,7 +1297,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1360,94 +1396,16 @@
     <xf numFmtId="14" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1469,26 +1427,101 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2278,717 +2311,752 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9AF0F5-701D-4995-8BE8-1AD93624257C}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="48" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-    </row>
-    <row r="3" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="49" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+    </row>
+    <row r="3" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="51" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="52" t="s">
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="54" t="s">
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="M4" s="55"/>
-      <c r="N4" s="56"/>
-    </row>
-    <row r="5" spans="1:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="64">
+      <c r="M4" s="60"/>
+      <c r="N4" s="61"/>
+    </row>
+    <row r="5" spans="1:14" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="62">
         <v>1</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="44" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44" t="s">
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44" t="s">
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77" t="s">
         <v>94</v>
       </c>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-    </row>
-    <row r="6" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="65"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-    </row>
-    <row r="8" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="64">
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+    </row>
+    <row r="6" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="63"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="64"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+    </row>
+    <row r="8" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="62">
         <v>2</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="45" t="s">
+      <c r="C8" s="52"/>
+      <c r="D8" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45" t="s">
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45" t="s">
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-    </row>
-    <row r="9" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="65"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-    </row>
-    <row r="11" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="64">
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+    </row>
+    <row r="9" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="63"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="64"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="75"/>
+    </row>
+    <row r="11" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="62">
         <v>3</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="45" t="s">
-        <v>128</v>
-      </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45" t="s">
+      <c r="C11" s="52"/>
+      <c r="D11" s="78" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78" t="s">
         <v>100</v>
       </c>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-    </row>
-    <row r="12" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="65"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-    </row>
-    <row r="14" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="57">
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="78"/>
+    </row>
+    <row r="12" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="63"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="78"/>
+    </row>
+    <row r="13" spans="1:14" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="64"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="78"/>
+      <c r="N13" s="78"/>
+    </row>
+    <row r="14" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="65">
         <v>4</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="52"/>
+      <c r="D14" s="75" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="75"/>
+      <c r="N14" s="75"/>
+    </row>
+    <row r="15" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="66"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="75"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="75"/>
+    </row>
+    <row r="16" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="67"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="75"/>
+      <c r="M16" s="75"/>
+      <c r="N16" s="75"/>
+    </row>
+    <row r="17" spans="1:14" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39">
+        <v>6</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="52"/>
+      <c r="D17" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="75" t="s">
+        <v>147</v>
+      </c>
+      <c r="I17" s="75"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="M17" s="79"/>
+      <c r="N17" s="79"/>
+    </row>
+    <row r="18" spans="1:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="39">
+        <v>7</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="52"/>
+      <c r="D18" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+    </row>
+    <row r="19" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="68">
+        <v>8</v>
+      </c>
+      <c r="B19" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="52"/>
+      <c r="D19" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75" t="s">
+        <v>151</v>
+      </c>
+      <c r="I19" s="75"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="75"/>
+      <c r="N19" s="75"/>
+    </row>
+    <row r="20" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="69"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="75"/>
+      <c r="N20" s="75"/>
+    </row>
+    <row r="21" spans="1:14" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="70"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="76"/>
+    </row>
+    <row r="22" spans="1:14" ht="61.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="39">
+        <v>10</v>
+      </c>
+      <c r="B22" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="75" t="s">
+        <v>154</v>
+      </c>
+      <c r="I22" s="75"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="75"/>
+      <c r="L22" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+    </row>
+    <row r="23" spans="1:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="39">
+        <v>11</v>
+      </c>
+      <c r="B23" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="52"/>
+      <c r="D23" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="79"/>
+    </row>
+    <row r="24" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="65">
+        <v>12</v>
+      </c>
+      <c r="B24" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45" t="s">
+      <c r="C24" s="52"/>
+      <c r="D24" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45" t="s">
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-    </row>
-    <row r="15" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="58"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="67"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-    </row>
-    <row r="17" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="60">
-        <v>5</v>
-      </c>
-      <c r="B17" s="43" t="s">
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="78"/>
+      <c r="M24" s="78"/>
+      <c r="N24" s="78"/>
+    </row>
+    <row r="25" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="66"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+    </row>
+    <row r="26" spans="1:14" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="72"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="78"/>
+    </row>
+    <row r="27" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="68">
+        <v>13</v>
+      </c>
+      <c r="B27" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45" t="s">
+      <c r="C27" s="52"/>
+      <c r="D27" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45" t="s">
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-    </row>
-    <row r="18" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="61"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="63"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-    </row>
-    <row r="20" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="57">
-        <v>6</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="45" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-    </row>
-    <row r="21" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-    </row>
-    <row r="23" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="60">
-        <v>7</v>
-      </c>
-      <c r="B23" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-    </row>
-    <row r="24" spans="1:15" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="61"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="62"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-    </row>
-    <row r="26" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="57">
-        <v>8</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47"/>
-    </row>
-    <row r="27" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="58"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
-    </row>
-    <row r="28" spans="1:15" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="77">
-        <v>9</v>
-      </c>
-      <c r="B29" s="76" t="s">
-        <v>137</v>
-      </c>
-      <c r="C29" s="76"/>
-      <c r="D29" s="75" t="s">
-        <v>140</v>
-      </c>
+      <c r="M27" s="78"/>
+      <c r="N27" s="78"/>
+    </row>
+    <row r="28" spans="1:14" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="69"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="75"/>
+      <c r="L28" s="78"/>
+      <c r="M28" s="78"/>
+      <c r="N28" s="78"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="73"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="75"/>
       <c r="E29" s="75"/>
       <c r="F29" s="75"/>
       <c r="G29" s="75"/>
-      <c r="H29" s="81" t="s">
-        <v>147</v>
-      </c>
+      <c r="H29" s="75"/>
       <c r="I29" s="75"/>
       <c r="J29" s="75"/>
       <c r="K29" s="75"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="75"/>
-      <c r="N29" s="75"/>
-    </row>
-    <row r="30" spans="1:15" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="77">
-        <v>10</v>
-      </c>
-      <c r="B30" s="76" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="76"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="78"/>
+    </row>
+    <row r="30" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="65">
+        <v>14</v>
+      </c>
+      <c r="B30" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="52"/>
       <c r="D30" s="75" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="E30" s="75"/>
       <c r="F30" s="75"/>
       <c r="G30" s="75"/>
-      <c r="H30" s="81" t="s">
-        <v>149</v>
+      <c r="H30" s="75" t="s">
+        <v>136</v>
       </c>
       <c r="I30" s="75"/>
       <c r="J30" s="75"/>
       <c r="K30" s="75"/>
-      <c r="L30" s="81" t="s">
-        <v>141</v>
+      <c r="L30" s="75" t="s">
+        <v>137</v>
       </c>
       <c r="M30" s="75"/>
       <c r="N30" s="75"/>
     </row>
-    <row r="31" spans="1:15" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="77">
-        <v>11</v>
-      </c>
-      <c r="B31" s="76" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="76"/>
-      <c r="D31" s="81" t="s">
-        <v>142</v>
-      </c>
-      <c r="E31" s="81"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="81" t="s">
-        <v>150</v>
-      </c>
+    <row r="31" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="66"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="75"/>
       <c r="I31" s="75"/>
       <c r="J31" s="75"/>
       <c r="K31" s="75"/>
-      <c r="L31" s="81" t="s">
-        <v>143</v>
-      </c>
+      <c r="L31" s="75"/>
       <c r="M31" s="75"/>
       <c r="N31" s="75"/>
     </row>
-    <row r="32" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="78">
-        <v>9</v>
-      </c>
-      <c r="B32" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-    </row>
-    <row r="33" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="79"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="47"/>
-    </row>
-    <row r="34" spans="1:15" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="80"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="45"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
-      <c r="O34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
+    <row r="32" spans="1:14" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="72"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="75"/>
+      <c r="M32" s="75"/>
+      <c r="N32" s="75"/>
+    </row>
+    <row r="33" spans="1:14" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="39">
+        <v>15</v>
+      </c>
+      <c r="B33" s="74" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="74"/>
+      <c r="D33" s="80" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="75" t="s">
+        <v>138</v>
+      </c>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+    </row>
+    <row r="34" spans="1:14" ht="82.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="39">
+        <v>16</v>
+      </c>
+      <c r="B34" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="74"/>
+      <c r="D34" s="75" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75" t="s">
+        <v>140</v>
+      </c>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="M34" s="75"/>
+      <c r="N34" s="75"/>
+    </row>
+    <row r="35" spans="1:14" ht="70.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="39">
+        <v>17</v>
+      </c>
+      <c r="B35" s="74" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="74"/>
+      <c r="D35" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" s="75"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="I35" s="75"/>
+      <c r="J35" s="75"/>
+      <c r="K35" s="75"/>
+      <c r="L35" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="M35" s="75"/>
+      <c r="N35" s="75"/>
+    </row>
+    <row r="36" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="68">
+        <v>18</v>
+      </c>
+      <c r="B36" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="52"/>
+      <c r="D36" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="I36" s="75"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="75"/>
+      <c r="L36" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="M36" s="75"/>
+      <c r="N36" s="75"/>
+    </row>
+    <row r="37" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="69"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="75"/>
+    </row>
+    <row r="38" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="70"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="75"/>
+      <c r="I38" s="75"/>
+      <c r="J38" s="75"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="75"/>
+      <c r="M38" s="75"/>
+      <c r="N38" s="75"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="B26:C28"/>
-    <mergeCell ref="D26:G28"/>
-    <mergeCell ref="H26:K28"/>
-    <mergeCell ref="L26:N28"/>
-    <mergeCell ref="B32:C34"/>
-    <mergeCell ref="D32:G34"/>
-    <mergeCell ref="H32:K34"/>
-    <mergeCell ref="L32:N34"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="B20:C22"/>
-    <mergeCell ref="D20:G22"/>
-    <mergeCell ref="H20:K22"/>
-    <mergeCell ref="L20:N22"/>
-    <mergeCell ref="B23:C25"/>
-    <mergeCell ref="D23:G25"/>
-    <mergeCell ref="H23:K25"/>
-    <mergeCell ref="L23:N25"/>
-    <mergeCell ref="B14:C16"/>
-    <mergeCell ref="D14:G16"/>
-    <mergeCell ref="H14:K16"/>
-    <mergeCell ref="L14:N16"/>
-    <mergeCell ref="B17:C19"/>
-    <mergeCell ref="D17:G19"/>
-    <mergeCell ref="H17:K19"/>
-    <mergeCell ref="L17:N19"/>
-    <mergeCell ref="B8:C10"/>
-    <mergeCell ref="D8:G10"/>
-    <mergeCell ref="H8:K10"/>
-    <mergeCell ref="L8:N10"/>
-    <mergeCell ref="B11:C13"/>
-    <mergeCell ref="D11:G13"/>
-    <mergeCell ref="H11:K13"/>
-    <mergeCell ref="L11:N13"/>
+  <mergeCells count="78">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B5:C7"/>
     <mergeCell ref="D5:G7"/>
     <mergeCell ref="H5:K7"/>
@@ -2998,6 +3066,67 @@
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
+    <mergeCell ref="B8:C10"/>
+    <mergeCell ref="D8:G10"/>
+    <mergeCell ref="H8:K10"/>
+    <mergeCell ref="L8:N10"/>
+    <mergeCell ref="B11:C13"/>
+    <mergeCell ref="D11:G13"/>
+    <mergeCell ref="H11:K13"/>
+    <mergeCell ref="L11:N13"/>
+    <mergeCell ref="B14:C16"/>
+    <mergeCell ref="D14:G16"/>
+    <mergeCell ref="H14:K16"/>
+    <mergeCell ref="L14:N16"/>
+    <mergeCell ref="B19:C21"/>
+    <mergeCell ref="D19:G21"/>
+    <mergeCell ref="H19:K21"/>
+    <mergeCell ref="L19:N21"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D24:G26"/>
+    <mergeCell ref="H24:K26"/>
+    <mergeCell ref="L24:N26"/>
+    <mergeCell ref="B27:C29"/>
+    <mergeCell ref="D27:G29"/>
+    <mergeCell ref="H27:K29"/>
+    <mergeCell ref="L27:N29"/>
+    <mergeCell ref="B36:C38"/>
+    <mergeCell ref="D36:G38"/>
+    <mergeCell ref="H36:K38"/>
+    <mergeCell ref="L36:N38"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B30:C32"/>
+    <mergeCell ref="D30:G32"/>
+    <mergeCell ref="H30:K32"/>
+    <mergeCell ref="L30:N32"/>
+    <mergeCell ref="B24:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3013,7 +3142,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -3068,14 +3197,14 @@
       <c r="W1" s="26"/>
     </row>
     <row r="2" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
@@ -3095,12 +3224,12 @@
       <c r="W2" s="27"/>
     </row>
     <row r="3" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
@@ -3120,12 +3249,12 @@
       <c r="W3" s="27"/>
     </row>
     <row r="4" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="68"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
       <c r="I4" s="27"/>
@@ -3145,16 +3274,16 @@
       <c r="W4" s="27"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="70"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="36"/>
-      <c r="D5" s="72" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="73"/>
-      <c r="F5" s="74"/>
+      <c r="D5" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
@@ -3181,34 +3310,34 @@
     </row>
     <row r="7" spans="1:45" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:45" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="69" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69" t="s">
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69" t="s">
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
-      <c r="U8" s="69"/>
-      <c r="V8" s="69"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
     </row>
     <row r="9" spans="1:45" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
@@ -3311,22 +3440,22 @@
         <v>0</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="11"/>
@@ -3355,22 +3484,22 @@
         <v>40</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>123</v>
-      </c>
       <c r="G12" s="22" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="11"/>
@@ -3399,22 +3528,22 @@
         <v>41</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C13" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>127</v>
-      </c>
       <c r="G13" s="22" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="11"/>
@@ -3447,7 +3576,7 @@
       <c r="D14" s="17"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
@@ -5814,6 +5943,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -5939,24 +6085,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5972,22 +6119,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TP11 actualizado con el TP12
</commit_message>
<xml_diff>
--- a/Practico/TPs/TP11/Resolucion-TP11-Ezequiel.xlsx
+++ b/Practico/TPs/TP11/Resolucion-TP11-Ezequiel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USUARIOS\FEDE\Documents\QUINTO AÑO\Ingenieria de Software\ISW-Grupo2-4K2-2022\Practico\TPs\TP11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gordo\UTN\Ingenieria de Software - 4K2\ISW-Grupo2-4K2-2022\Practico\TPs\TP11\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCB1A92-2BEE-4501-AE36-1EFAF2DC3488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="679" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="679" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla de Test - Caja Negra" sheetId="29" r:id="rId1"/>
@@ -24,12 +25,12 @@
     <definedName name="Ready_To_Run">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr autoRecover="0" repairLoad="1"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="161">
   <si>
     <t>TC_001</t>
   </si>
@@ -478,15 +479,6 @@
     <t>Errores del formulario de pedido</t>
   </si>
   <si>
-    <t>1- el comprador selecciona "Realizar Pedido de lo que sea"
-2- el comprador no ingresa descripcion del producto
-3- El comprador sube una foto de mas de 5 MB
-4- El comprador no selecciona ninguna ciudad
-5- El comprador no ingresa la calle y la altura de la direccion de comercio
-6- El comprador no ingresa la calle y altura de la direccion de entrega
-7- El comprador selecciona la opcion "confirmar destino"</t>
-  </si>
-  <si>
     <t>1- el sistema muestra el formulario de pedido a llenar
 2- El sistema muestra un mensaje de error por no ingresar la descripcion del producto
 3- E l sistema muestra un mensaje de error por ingresar una foto no valida
@@ -519,6 +511,155 @@
     <t>Errores en la forma de pago por tarjeta (numero de tarjeta, CVV y fechas invalidas)</t>
   </si>
   <si>
+    <t>1- el sistema muestra el formulario de pedido a llenar
+6- el sistema muestra el monto y el formulario de forma de pago a llenar
+8-El sistema muestra un mensaje de error por no ingresar el numero de tarjeta
+8-El sistema muestra un mensaje de error por no ingresar nombre y apellido del titular
+8- El sistema muestra un mensaje de error por no ingresar un CVV
+8- El sistema muestra un mensaje de error por no ingresar fecha de vencimiento
+10- El sistema solicita que se revisen los campos con errores</t>
+  </si>
+  <si>
+    <t>1- el sistema muestra el formulario de pedido a llenar
+6- el sistema muestra el monto y el formulario de forma de pago a llenar
+8-El sistema muestra un mensaje de error por ingresar un numero de trajeta no valido
+9- El sistema muestra un mensaje de error por ingresar un CVV no valido
+10- El sistema muestra un mensaje de error por tarjeta vencida
+11- El sistema muestra un mensaje de error por ingresar una fecha de entrega no valida
+12- El sistema solicita que se revisen los campos con errores</t>
+  </si>
+  <si>
+    <t>Errores en la forma de pago por efectivo</t>
+  </si>
+  <si>
+    <t>La ciudad Cordoba esta cargada en la app
+Precio de envio: $300 por metro lineal + un costo base de $500
+Las direcciones "Juan B Justo 1234" y "Mariano Fragueiro 1122" son de Cordoba</t>
+  </si>
+  <si>
+    <t>1- el comprador selecciona "Realizar Pedido de lo que sea"
+2- el comprador ingresa en el campo de texto la especifiacion del producto: "Gorra Adidas Negra"
+3- El comprador selecciona la ciudad: "Cordoba"
+4- El comprador ingresa en el campo de texto la direccion del comercio sin referencia: "Juan B Justo 1234"
+5-  El comprador ingresa la direccion de entrega sin referencia: "Mariano Fragueiro 1122"
+6- El comprador selecciona "confirmar destino"
+7- el comprador selecciona "Efectivo" como forma de pago
+8- el comprador ingresa el monto 50
+9- el comprador selecciona entrega "Lo antes posible"
+10- El comprador confirma la finalizacion del pedido</t>
+  </si>
+  <si>
+    <t>1- el sistema muestra el formulario de pedido a llenar
+6- el sistema muestra el monto y el formulario de forma de pago a llenar
+8-El sistema muestra un mensaje de error por ingresar un monto inferior al necesario
+10- El sistema solicita que se revisen los campos con errores</t>
+  </si>
+  <si>
+    <t>1-2-3-4-5-6-7-8-9-10-11-12-13-18</t>
+  </si>
+  <si>
+    <t>1-3-4-5-7-8-12-14-15-16-17</t>
+  </si>
+  <si>
+    <t>NINGUNO</t>
+  </si>
+  <si>
+    <t>permite subir imagen de otro formato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- el compador sube una imagen del producto en formato ".png" </t>
+  </si>
+  <si>
+    <t>Severo</t>
+  </si>
+  <si>
+    <t>Creado</t>
+  </si>
+  <si>
+    <t>Cosmetico</t>
+  </si>
+  <si>
+    <t>Paso</t>
+  </si>
+  <si>
+    <t>1- el comprador selecciona "Realizar Pedido de lo que sea"
+2- el comprador no ingresa descripcion del producto
+3- El comprador sube una foto de mas de 5 MB y de otro formato
+4- El comprador no selecciona ninguna ciudad
+5- El comprador no ingresa la calle y la altura de la direccion de comercio
+6- El comprador no ingresa la calle y altura de la direccion de entrega
+7- El comprador selecciona la opcion "confirmar destino"</t>
+  </si>
+  <si>
+    <t>1- el sistema muestra el formulario de pedido a llenar
+2- el sistema muestra el formulario de pedido a llenar
+3- E l sistema muestra un mensaje de error por ingresar una foto de menor tamaño, pero permite ingresar con otro formato
+4- el sistema muestra el formulario de pedido a llenar
+5- el sistema muestra el formulario de pedido a llenarla direccion del comercio
+6- el sistema muestra el formulario de pedido a llenar
+7- El sistema solicita que se revisen los campos con errores</t>
+  </si>
+  <si>
+    <t>el campo de piso de la direccion de entrega acepta caracteres "+" ó "-"</t>
+  </si>
+  <si>
+    <t>1- el compador agrega "+" y/o "-" en el piso de la direccion de entrega</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>acepta fecha menor a la fecha actual en la fecha de entrega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- el comprador elige la fecha de entrega "25/10/2010 14:23" </t>
+  </si>
+  <si>
+    <t>acepta fecha mayor a 7 dias de la fecha actual en la fecha de entrega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- el comprador elige la fecha de entrega "03/11/2010 14:25" </t>
+  </si>
+  <si>
+    <t>acepta fecha de vencimiento de tarjetas menores a la fecha actual (Descripcion: "permite hasta 08 del 2022")</t>
+  </si>
+  <si>
+    <t>1- el comprador elige fecha de vencimiento de la tarjeta como "08/2022"</t>
+  </si>
+  <si>
+    <t>Critico</t>
+  </si>
+  <si>
+    <t>permite escribir caracteres alfanumericos en el monto de efectivo</t>
+  </si>
+  <si>
+    <t>1- el comprador ingresa "2500ag" en el monto de efectivo</t>
+  </si>
+  <si>
+    <t>1- el comprador no elige la ciudad
+2- el comprador ingresa "juan montalvo 3344" como direccion de destino
+3- el comprador ingresa "Mexico 123" como direccion de entrega
+4- el comprador confirma destino</t>
+  </si>
+  <si>
+    <t>1- el sistema muestra el formulario de pedido a llenar
+6- el sistema muestra el monto y el formulario de forma de pago a llenar
+8-El sistema muestra un mensaje de error por ingresar un monto inferior al necesario, pero si ingresa carateres alfanumericos, lo pasa
+10- El sistema solicita que se revisen los campos con errores</t>
+  </si>
+  <si>
+    <t>1- el sistema muestra el formulario de pedido a llenar
+6- el sistema muestra el monto y el formulario de forma de pago a llenar
+8-El sistema muestra un mensaje de error por ingresar un numero de trajeta no valido
+9- El sistema muestra un mensaje de error por ingresar un CVV no valido
+10- El sistema permite elegir fecha de vencimiento anteriores de la actual
+11- El sistema permite elegir fechas anteriores a la fecha actual
+12- El sistema solicita que se revisen los campos con errores</t>
+  </si>
+  <si>
+    <t>Ingresar fecha de entrega mayor a 7 dias de la fecha cuando se realiza el pedido</t>
+  </si>
+  <si>
     <t>1- el comprador selecciona "Realizar Pedido de lo que sea"
 2- el comprador ingresa en el campo de texto la especifiacion del producto: "Gorra Adidas Negra"
 3- El comprador selecciona la ciudad: "Cordoba"
@@ -529,34 +670,8 @@
 8- el comprador ingresa el numero de tarjeta 1111 2222 3333 444
 9- el comprador ingresa el CVV 1111
 10- el comprador ingresa la fecha de vencimiento 08/2022
-11- el comprador ingresa la fecha de entrega 5/11/2022 13:3010
+11- el comprador ingresa la fecha de entrega 5/10/2010 13:30
 12- El comprador confirma la finalizacion del pedido</t>
-  </si>
-  <si>
-    <t>1- el sistema muestra el formulario de pedido a llenar
-6- el sistema muestra el monto y el formulario de forma de pago a llenar
-8-El sistema muestra un mensaje de error por no ingresar el numero de tarjeta
-8-El sistema muestra un mensaje de error por no ingresar nombre y apellido del titular
-8- El sistema muestra un mensaje de error por no ingresar un CVV
-8- El sistema muestra un mensaje de error por no ingresar fecha de vencimiento
-10- El sistema solicita que se revisen los campos con errores</t>
-  </si>
-  <si>
-    <t>1- el sistema muestra el formulario de pedido a llenar
-6- el sistema muestra el monto y el formulario de forma de pago a llenar
-8-El sistema muestra un mensaje de error por ingresar un numero de trajeta no valido
-9- El sistema muestra un mensaje de error por ingresar un CVV no valido
-10- El sistema muestra un mensaje de error por tarjeta vencida
-11- El sistema muestra un mensaje de error por ingresar una fecha de entrega no valida
-12- El sistema solicita que se revisen los campos con errores</t>
-  </si>
-  <si>
-    <t>Errores en la forma de pago por efectivo</t>
-  </si>
-  <si>
-    <t>La ciudad Cordoba esta cargada en la app
-Precio de envio: $300 por metro lineal + un costo base de $500
-Las direcciones "Juan B Justo 1234" y "Mariano Fragueiro 1122" son de Cordoba</t>
   </si>
   <si>
     <t>1- el comprador selecciona "Realizar Pedido de lo que sea"
@@ -566,27 +681,48 @@
 5-  El comprador ingresa la direccion de entrega sin referencia: "Mariano Fragueiro 1122"
 6- El comprador selecciona "confirmar destino"
 7- el comprador selecciona "Efectivo" como forma de pago
-8- el comprador ingresa el monto 50
-9- el comprador selecciona entrega "Lo antes posible"
-10- El comprador confirma la finalizacion del pedido</t>
+8- el comprador ingresa el monto mayor al monto total
+9- el comprador selecciona entrega "fecha proramada"
+10- el comprador selecciona la fecha "05/11/2022 14:30"
+11- El comprador confirma la finalizacion del pedido</t>
   </si>
   <si>
     <t>1- el sistema muestra el formulario de pedido a llenar
 6- el sistema muestra el monto y el formulario de forma de pago a llenar
 8-El sistema muestra un mensaje de error por ingresar un monto inferior al necesario
-10- El sistema solicita que se revisen los campos con errores</t>
-  </si>
-  <si>
-    <t>1-2-3-4-5-6-7-8-9-10-11-12-13-18</t>
-  </si>
-  <si>
-    <t>1-3-4-5-7-8-12-14-15-16-17</t>
+10- El sistema advierte que la fecha de entrega supera el plazo de 7 dias
+11- El sistema solicita que se revisen los campos con errores</t>
+  </si>
+  <si>
+    <t>1- el sistema muestra el formulario de pedido a llenar
+6- el sistema muestra el monto y el formulario de forma de pago a llenar
+8-El sistema muestra un mensaje de error por ingresar un monto inferior al necesario, pero si ingresa carateres alfanumericos, lo pasa
+10- El sistema no avisa que la fecha de entrega supera el plazo de 7 dias
+11- El sistema solicita que se revisen los campos con errores</t>
+  </si>
+  <si>
+    <t>no avisa que no elegiste ciudad cuando confirmas el destino</t>
+  </si>
+  <si>
+    <t>el campo nro de direccion de entrega no muestra error por exceso de caracteres, sino que solicita que ingrese un numero valido</t>
+  </si>
+  <si>
+    <t>el campo nro de direccion de comercio no muestra error por exceso de caracteres, sino que solicita que ingrese un numero valido</t>
+  </si>
+  <si>
+    <t>1- el comprador ingresa "12324221232422123242212324221232422123242212324221232422"en el campo de entrega</t>
+  </si>
+  <si>
+    <t>1- el comprador ingresa "12324221232422123242212324221232422123242212324221232422"en el campo de comercio</t>
+  </si>
+  <si>
+    <t>TC_008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -794,7 +930,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1344,6 +1480,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1361,7 +1534,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1649,6 +1822,15 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1658,15 +1840,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1697,20 +1870,150 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="DataPilot Category" xfId="1"/>
-    <cellStyle name="DataPilot Corner" xfId="2"/>
-    <cellStyle name="DataPilot Field" xfId="3"/>
-    <cellStyle name="DataPilot Result" xfId="4"/>
-    <cellStyle name="DataPilot Title" xfId="5"/>
-    <cellStyle name="DataPilot Value" xfId="6"/>
+    <cellStyle name="DataPilot Category" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="DataPilot Corner" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="DataPilot Field" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="DataPilot Result" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="DataPilot Title" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="DataPilot Value" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="8"/>
+    <cellStyle name="Normal 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Total" xfId="9" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="47">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1976,55 +2279,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="34"/>
           <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2484,10 +2738,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N76"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="B35" sqref="B35:C35"/>
     </sheetView>
   </sheetViews>
@@ -3967,15 +4221,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AS73"/>
+  <dimension ref="A1:AS87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60:C73"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F74" sqref="F74:F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4004,7 +4258,7 @@
     <col min="23" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25"/>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -4135,13 +4389,13 @@
       <c r="V5" s="27"/>
       <c r="W5" s="27"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="M6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:45" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:45" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:45" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="113"/>
       <c r="B8" s="113"/>
@@ -4276,7 +4530,7 @@
         <v>54</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>103</v>
@@ -4290,16 +4544,32 @@
       <c r="G11" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="11"/>
+      <c r="H11" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="J11" s="24"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="23"/>
+      <c r="K11" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" s="117">
+        <v>44859.569444444445</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>132</v>
+      </c>
       <c r="O11" s="24"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="31"/>
+      <c r="P11" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q11" s="118">
+        <v>44859.57708333333</v>
+      </c>
       <c r="R11" s="11"/>
       <c r="S11" s="23"/>
       <c r="T11" s="24"/>
@@ -4320,7 +4590,7 @@
         <v>54</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>108</v>
@@ -4334,16 +4604,32 @@
       <c r="G12" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="11"/>
+      <c r="H12" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="J12" s="23"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="11"/>
+      <c r="K12" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="L12" s="29">
+        <v>44859.576388888891</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="O12" s="23"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="12"/>
+      <c r="P12" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q12" s="118">
+        <v>44859.578472222223</v>
+      </c>
       <c r="R12" s="31"/>
       <c r="S12" s="11"/>
       <c r="T12" s="23"/>
@@ -4364,7 +4650,7 @@
         <v>54</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>107</v>
@@ -4378,16 +4664,32 @@
       <c r="G13" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="11"/>
+      <c r="H13" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="J13" s="23"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="11"/>
+      <c r="K13" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="L13" s="29">
+        <v>44859.582638888889</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="O13" s="23"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="12"/>
+      <c r="P13" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q13" s="29">
+        <v>44859.586805555555</v>
+      </c>
       <c r="R13" s="31"/>
       <c r="S13" s="11"/>
       <c r="T13" s="23"/>
@@ -4400,7 +4702,7 @@
       <c r="AR13" s="4"/>
       <c r="AS13" s="4"/>
     </row>
-    <row r="14" spans="1:45" ht="144" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="300" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>3</v>
       </c>
@@ -4414,24 +4716,40 @@
         <v>112</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F14" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="11"/>
+      <c r="H14" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="J14" s="23"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="11"/>
+      <c r="K14" s="24">
+        <v>2</v>
+      </c>
+      <c r="L14" s="29">
+        <v>44859.586111111108</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="O14" s="23"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="12"/>
+      <c r="P14" s="24">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="29">
+        <v>44859.586111111108</v>
+      </c>
       <c r="R14" s="31"/>
       <c r="S14" s="11"/>
       <c r="T14" s="23"/>
@@ -4445,37 +4763,53 @@
       <c r="AS14" s="4"/>
     </row>
     <row r="15" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="104" t="s">
         <v>111</v>
       </c>
       <c r="C15" s="98">
         <v>19</v>
       </c>
       <c r="D15" s="98" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E15" s="107" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F15" s="95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G15" s="95" t="s">
-        <v>120</v>
-      </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="12"/>
+        <v>118</v>
+      </c>
+      <c r="H15" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="I15" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J15" s="123"/>
+      <c r="K15" s="126" t="s">
+        <v>126</v>
+      </c>
+      <c r="L15" s="129">
+        <v>44859.59375</v>
+      </c>
+      <c r="M15" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="N15" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="O15" s="123"/>
+      <c r="P15" s="126" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q15" s="129">
+        <v>44859.600694444445</v>
+      </c>
       <c r="R15" s="31"/>
       <c r="S15" s="11"/>
       <c r="T15" s="23"/>
@@ -4489,23 +4823,23 @@
       <c r="AS15" s="4"/>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A16" s="105"/>
-      <c r="B16" s="102"/>
+      <c r="A16" s="102"/>
+      <c r="B16" s="105"/>
       <c r="C16" s="99"/>
       <c r="D16" s="99"/>
       <c r="E16" s="108"/>
       <c r="F16" s="96"/>
       <c r="G16" s="96"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="12"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="124"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="130"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="121"/>
+      <c r="O16" s="124"/>
+      <c r="P16" s="127"/>
+      <c r="Q16" s="130"/>
       <c r="R16" s="31"/>
       <c r="S16" s="11"/>
       <c r="T16" s="23"/>
@@ -4519,23 +4853,23 @@
       <c r="AS16" s="4"/>
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A17" s="105"/>
-      <c r="B17" s="102"/>
+      <c r="A17" s="102"/>
+      <c r="B17" s="105"/>
       <c r="C17" s="99"/>
       <c r="D17" s="99"/>
       <c r="E17" s="108"/>
       <c r="F17" s="96"/>
       <c r="G17" s="96"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="12"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="124"/>
+      <c r="K17" s="127"/>
+      <c r="L17" s="130"/>
+      <c r="M17" s="96"/>
+      <c r="N17" s="121"/>
+      <c r="O17" s="124"/>
+      <c r="P17" s="127"/>
+      <c r="Q17" s="130"/>
       <c r="R17" s="31"/>
       <c r="S17" s="11"/>
       <c r="T17" s="23"/>
@@ -4549,23 +4883,23 @@
       <c r="AS17" s="4"/>
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A18" s="105"/>
-      <c r="B18" s="102"/>
+      <c r="A18" s="102"/>
+      <c r="B18" s="105"/>
       <c r="C18" s="99"/>
       <c r="D18" s="99"/>
       <c r="E18" s="108"/>
       <c r="F18" s="96"/>
       <c r="G18" s="96"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="12"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="124"/>
+      <c r="K18" s="127"/>
+      <c r="L18" s="130"/>
+      <c r="M18" s="96"/>
+      <c r="N18" s="121"/>
+      <c r="O18" s="124"/>
+      <c r="P18" s="127"/>
+      <c r="Q18" s="130"/>
       <c r="R18" s="31"/>
       <c r="S18" s="11"/>
       <c r="T18" s="23"/>
@@ -4579,23 +4913,23 @@
       <c r="AS18" s="4"/>
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A19" s="105"/>
-      <c r="B19" s="102"/>
+      <c r="A19" s="102"/>
+      <c r="B19" s="105"/>
       <c r="C19" s="99"/>
       <c r="D19" s="99"/>
       <c r="E19" s="108"/>
       <c r="F19" s="96"/>
       <c r="G19" s="96"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="12"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="121"/>
+      <c r="J19" s="124"/>
+      <c r="K19" s="127"/>
+      <c r="L19" s="130"/>
+      <c r="M19" s="96"/>
+      <c r="N19" s="121"/>
+      <c r="O19" s="124"/>
+      <c r="P19" s="127"/>
+      <c r="Q19" s="130"/>
       <c r="R19" s="31"/>
       <c r="S19" s="11"/>
       <c r="T19" s="23"/>
@@ -4609,23 +4943,23 @@
       <c r="AS19" s="4"/>
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A20" s="105"/>
-      <c r="B20" s="102"/>
+      <c r="A20" s="102"/>
+      <c r="B20" s="105"/>
       <c r="C20" s="99"/>
       <c r="D20" s="99"/>
       <c r="E20" s="108"/>
       <c r="F20" s="96"/>
       <c r="G20" s="96"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="12"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="121"/>
+      <c r="J20" s="124"/>
+      <c r="K20" s="127"/>
+      <c r="L20" s="130"/>
+      <c r="M20" s="96"/>
+      <c r="N20" s="121"/>
+      <c r="O20" s="124"/>
+      <c r="P20" s="127"/>
+      <c r="Q20" s="130"/>
       <c r="R20" s="31"/>
       <c r="S20" s="11"/>
       <c r="T20" s="23"/>
@@ -4639,23 +4973,23 @@
       <c r="AS20" s="4"/>
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A21" s="105"/>
-      <c r="B21" s="102"/>
+      <c r="A21" s="102"/>
+      <c r="B21" s="105"/>
       <c r="C21" s="99"/>
       <c r="D21" s="99"/>
       <c r="E21" s="108"/>
       <c r="F21" s="96"/>
       <c r="G21" s="96"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="12"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="121"/>
+      <c r="J21" s="124"/>
+      <c r="K21" s="127"/>
+      <c r="L21" s="130"/>
+      <c r="M21" s="96"/>
+      <c r="N21" s="121"/>
+      <c r="O21" s="124"/>
+      <c r="P21" s="127"/>
+      <c r="Q21" s="130"/>
       <c r="R21" s="31"/>
       <c r="S21" s="11"/>
       <c r="T21" s="23"/>
@@ -4669,23 +5003,23 @@
       <c r="AS21" s="4"/>
     </row>
     <row r="22" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A22" s="105"/>
-      <c r="B22" s="102"/>
+      <c r="A22" s="102"/>
+      <c r="B22" s="105"/>
       <c r="C22" s="99"/>
       <c r="D22" s="99"/>
       <c r="E22" s="108"/>
       <c r="F22" s="96"/>
       <c r="G22" s="96"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="12"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="121"/>
+      <c r="J22" s="124"/>
+      <c r="K22" s="127"/>
+      <c r="L22" s="130"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="121"/>
+      <c r="O22" s="124"/>
+      <c r="P22" s="127"/>
+      <c r="Q22" s="130"/>
       <c r="R22" s="31"/>
       <c r="S22" s="11"/>
       <c r="T22" s="23"/>
@@ -4699,23 +5033,23 @@
       <c r="AS22" s="4"/>
     </row>
     <row r="23" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A23" s="105"/>
-      <c r="B23" s="102"/>
+      <c r="A23" s="102"/>
+      <c r="B23" s="105"/>
       <c r="C23" s="99"/>
       <c r="D23" s="99"/>
       <c r="E23" s="108"/>
       <c r="F23" s="96"/>
       <c r="G23" s="96"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="12"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="121"/>
+      <c r="J23" s="124"/>
+      <c r="K23" s="127"/>
+      <c r="L23" s="130"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="121"/>
+      <c r="O23" s="124"/>
+      <c r="P23" s="127"/>
+      <c r="Q23" s="130"/>
       <c r="R23" s="31"/>
       <c r="S23" s="11"/>
       <c r="T23" s="23"/>
@@ -4729,23 +5063,23 @@
       <c r="AS23" s="4"/>
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A24" s="105"/>
-      <c r="B24" s="102"/>
+      <c r="A24" s="102"/>
+      <c r="B24" s="105"/>
       <c r="C24" s="99"/>
       <c r="D24" s="99"/>
       <c r="E24" s="108"/>
       <c r="F24" s="96"/>
       <c r="G24" s="96"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="12"/>
+      <c r="H24" s="96"/>
+      <c r="I24" s="121"/>
+      <c r="J24" s="124"/>
+      <c r="K24" s="127"/>
+      <c r="L24" s="130"/>
+      <c r="M24" s="96"/>
+      <c r="N24" s="121"/>
+      <c r="O24" s="124"/>
+      <c r="P24" s="127"/>
+      <c r="Q24" s="130"/>
       <c r="R24" s="31"/>
       <c r="S24" s="11"/>
       <c r="T24" s="23"/>
@@ -4759,23 +5093,23 @@
       <c r="AS24" s="4"/>
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A25" s="105"/>
-      <c r="B25" s="102"/>
+      <c r="A25" s="102"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="99"/>
       <c r="D25" s="99"/>
       <c r="E25" s="108"/>
       <c r="F25" s="96"/>
       <c r="G25" s="96"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="12"/>
+      <c r="H25" s="96"/>
+      <c r="I25" s="121"/>
+      <c r="J25" s="124"/>
+      <c r="K25" s="127"/>
+      <c r="L25" s="130"/>
+      <c r="M25" s="96"/>
+      <c r="N25" s="121"/>
+      <c r="O25" s="124"/>
+      <c r="P25" s="127"/>
+      <c r="Q25" s="130"/>
       <c r="R25" s="31"/>
       <c r="S25" s="11"/>
       <c r="T25" s="23"/>
@@ -4789,23 +5123,23 @@
       <c r="AS25" s="4"/>
     </row>
     <row r="26" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A26" s="105"/>
-      <c r="B26" s="102"/>
+      <c r="A26" s="102"/>
+      <c r="B26" s="105"/>
       <c r="C26" s="99"/>
       <c r="D26" s="99"/>
       <c r="E26" s="108"/>
       <c r="F26" s="96"/>
       <c r="G26" s="96"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="12"/>
+      <c r="H26" s="96"/>
+      <c r="I26" s="121"/>
+      <c r="J26" s="124"/>
+      <c r="K26" s="127"/>
+      <c r="L26" s="130"/>
+      <c r="M26" s="96"/>
+      <c r="N26" s="121"/>
+      <c r="O26" s="124"/>
+      <c r="P26" s="127"/>
+      <c r="Q26" s="130"/>
       <c r="R26" s="31"/>
       <c r="S26" s="11"/>
       <c r="T26" s="23"/>
@@ -4819,23 +5153,23 @@
       <c r="AS26" s="4"/>
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A27" s="105"/>
-      <c r="B27" s="102"/>
+      <c r="A27" s="102"/>
+      <c r="B27" s="105"/>
       <c r="C27" s="99"/>
       <c r="D27" s="99"/>
       <c r="E27" s="108"/>
       <c r="F27" s="96"/>
       <c r="G27" s="96"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="12"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="121"/>
+      <c r="J27" s="124"/>
+      <c r="K27" s="127"/>
+      <c r="L27" s="130"/>
+      <c r="M27" s="96"/>
+      <c r="N27" s="121"/>
+      <c r="O27" s="124"/>
+      <c r="P27" s="127"/>
+      <c r="Q27" s="130"/>
       <c r="R27" s="31"/>
       <c r="S27" s="11"/>
       <c r="T27" s="23"/>
@@ -4849,23 +5183,23 @@
       <c r="AS27" s="4"/>
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A28" s="105"/>
-      <c r="B28" s="102"/>
+      <c r="A28" s="102"/>
+      <c r="B28" s="105"/>
       <c r="C28" s="99"/>
       <c r="D28" s="99"/>
       <c r="E28" s="108"/>
       <c r="F28" s="96"/>
       <c r="G28" s="96"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="12"/>
+      <c r="H28" s="96"/>
+      <c r="I28" s="121"/>
+      <c r="J28" s="124"/>
+      <c r="K28" s="127"/>
+      <c r="L28" s="130"/>
+      <c r="M28" s="96"/>
+      <c r="N28" s="121"/>
+      <c r="O28" s="124"/>
+      <c r="P28" s="127"/>
+      <c r="Q28" s="130"/>
       <c r="R28" s="31"/>
       <c r="S28" s="11"/>
       <c r="T28" s="23"/>
@@ -4879,23 +5213,23 @@
       <c r="AS28" s="4"/>
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A29" s="105"/>
-      <c r="B29" s="102"/>
+      <c r="A29" s="102"/>
+      <c r="B29" s="105"/>
       <c r="C29" s="99"/>
       <c r="D29" s="99"/>
       <c r="E29" s="108"/>
       <c r="F29" s="96"/>
       <c r="G29" s="96"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="12"/>
+      <c r="H29" s="96"/>
+      <c r="I29" s="121"/>
+      <c r="J29" s="124"/>
+      <c r="K29" s="127"/>
+      <c r="L29" s="130"/>
+      <c r="M29" s="96"/>
+      <c r="N29" s="121"/>
+      <c r="O29" s="124"/>
+      <c r="P29" s="127"/>
+      <c r="Q29" s="130"/>
       <c r="R29" s="31"/>
       <c r="S29" s="11"/>
       <c r="T29" s="23"/>
@@ -4909,23 +5243,23 @@
       <c r="AS29" s="4"/>
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A30" s="105"/>
-      <c r="B30" s="102"/>
+      <c r="A30" s="102"/>
+      <c r="B30" s="105"/>
       <c r="C30" s="99"/>
       <c r="D30" s="99"/>
       <c r="E30" s="108"/>
       <c r="F30" s="96"/>
       <c r="G30" s="96"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="12"/>
+      <c r="H30" s="96"/>
+      <c r="I30" s="121"/>
+      <c r="J30" s="124"/>
+      <c r="K30" s="127"/>
+      <c r="L30" s="130"/>
+      <c r="M30" s="96"/>
+      <c r="N30" s="121"/>
+      <c r="O30" s="124"/>
+      <c r="P30" s="127"/>
+      <c r="Q30" s="130"/>
       <c r="R30" s="31"/>
       <c r="S30" s="11"/>
       <c r="T30" s="23"/>
@@ -4939,23 +5273,23 @@
       <c r="AS30" s="4"/>
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A31" s="105"/>
-      <c r="B31" s="102"/>
+      <c r="A31" s="102"/>
+      <c r="B31" s="105"/>
       <c r="C31" s="99"/>
       <c r="D31" s="99"/>
       <c r="E31" s="108"/>
       <c r="F31" s="96"/>
       <c r="G31" s="96"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="12"/>
+      <c r="H31" s="96"/>
+      <c r="I31" s="121"/>
+      <c r="J31" s="124"/>
+      <c r="K31" s="127"/>
+      <c r="L31" s="130"/>
+      <c r="M31" s="96"/>
+      <c r="N31" s="121"/>
+      <c r="O31" s="124"/>
+      <c r="P31" s="127"/>
+      <c r="Q31" s="130"/>
       <c r="R31" s="31"/>
       <c r="S31" s="11"/>
       <c r="T31" s="23"/>
@@ -4969,23 +5303,23 @@
       <c r="AS31" s="4"/>
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A32" s="105"/>
-      <c r="B32" s="102"/>
+      <c r="A32" s="102"/>
+      <c r="B32" s="105"/>
       <c r="C32" s="99"/>
       <c r="D32" s="99"/>
       <c r="E32" s="108"/>
       <c r="F32" s="96"/>
       <c r="G32" s="96"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="12"/>
+      <c r="H32" s="96"/>
+      <c r="I32" s="121"/>
+      <c r="J32" s="124"/>
+      <c r="K32" s="127"/>
+      <c r="L32" s="130"/>
+      <c r="M32" s="96"/>
+      <c r="N32" s="121"/>
+      <c r="O32" s="124"/>
+      <c r="P32" s="127"/>
+      <c r="Q32" s="130"/>
       <c r="R32" s="31"/>
       <c r="S32" s="11"/>
       <c r="T32" s="23"/>
@@ -4999,23 +5333,23 @@
       <c r="AS32" s="4"/>
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A33" s="105"/>
-      <c r="B33" s="102"/>
+      <c r="A33" s="102"/>
+      <c r="B33" s="105"/>
       <c r="C33" s="99"/>
       <c r="D33" s="99"/>
       <c r="E33" s="108"/>
       <c r="F33" s="96"/>
       <c r="G33" s="96"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="12"/>
+      <c r="H33" s="96"/>
+      <c r="I33" s="121"/>
+      <c r="J33" s="124"/>
+      <c r="K33" s="127"/>
+      <c r="L33" s="130"/>
+      <c r="M33" s="96"/>
+      <c r="N33" s="121"/>
+      <c r="O33" s="124"/>
+      <c r="P33" s="127"/>
+      <c r="Q33" s="130"/>
       <c r="R33" s="31"/>
       <c r="S33" s="11"/>
       <c r="T33" s="23"/>
@@ -5029,23 +5363,23 @@
       <c r="AS33" s="4"/>
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A34" s="105"/>
-      <c r="B34" s="102"/>
+      <c r="A34" s="102"/>
+      <c r="B34" s="105"/>
       <c r="C34" s="99"/>
       <c r="D34" s="99"/>
       <c r="E34" s="108"/>
       <c r="F34" s="96"/>
       <c r="G34" s="96"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="12"/>
+      <c r="H34" s="96"/>
+      <c r="I34" s="121"/>
+      <c r="J34" s="124"/>
+      <c r="K34" s="127"/>
+      <c r="L34" s="130"/>
+      <c r="M34" s="96"/>
+      <c r="N34" s="121"/>
+      <c r="O34" s="124"/>
+      <c r="P34" s="127"/>
+      <c r="Q34" s="130"/>
       <c r="R34" s="31"/>
       <c r="S34" s="11"/>
       <c r="T34" s="23"/>
@@ -5059,23 +5393,23 @@
       <c r="AS34" s="4"/>
     </row>
     <row r="35" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A35" s="105"/>
-      <c r="B35" s="102"/>
+      <c r="A35" s="102"/>
+      <c r="B35" s="105"/>
       <c r="C35" s="99"/>
       <c r="D35" s="99"/>
       <c r="E35" s="108"/>
       <c r="F35" s="96"/>
       <c r="G35" s="96"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="12"/>
+      <c r="H35" s="96"/>
+      <c r="I35" s="121"/>
+      <c r="J35" s="124"/>
+      <c r="K35" s="127"/>
+      <c r="L35" s="130"/>
+      <c r="M35" s="96"/>
+      <c r="N35" s="121"/>
+      <c r="O35" s="124"/>
+      <c r="P35" s="127"/>
+      <c r="Q35" s="130"/>
       <c r="R35" s="31"/>
       <c r="S35" s="11"/>
       <c r="T35" s="23"/>
@@ -5089,23 +5423,23 @@
       <c r="AS35" s="4"/>
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A36" s="105"/>
-      <c r="B36" s="102"/>
+      <c r="A36" s="102"/>
+      <c r="B36" s="105"/>
       <c r="C36" s="99"/>
       <c r="D36" s="99"/>
       <c r="E36" s="108"/>
       <c r="F36" s="96"/>
       <c r="G36" s="96"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="12"/>
+      <c r="H36" s="96"/>
+      <c r="I36" s="121"/>
+      <c r="J36" s="124"/>
+      <c r="K36" s="127"/>
+      <c r="L36" s="130"/>
+      <c r="M36" s="96"/>
+      <c r="N36" s="121"/>
+      <c r="O36" s="124"/>
+      <c r="P36" s="127"/>
+      <c r="Q36" s="130"/>
       <c r="R36" s="31"/>
       <c r="S36" s="11"/>
       <c r="T36" s="23"/>
@@ -5119,23 +5453,23 @@
       <c r="AS36" s="4"/>
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A37" s="106"/>
-      <c r="B37" s="103"/>
+      <c r="A37" s="103"/>
+      <c r="B37" s="106"/>
       <c r="C37" s="100"/>
       <c r="D37" s="100"/>
       <c r="E37" s="109"/>
       <c r="F37" s="97"/>
       <c r="G37" s="97"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="31"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="23"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="12"/>
+      <c r="H37" s="97"/>
+      <c r="I37" s="122"/>
+      <c r="J37" s="125"/>
+      <c r="K37" s="128"/>
+      <c r="L37" s="131"/>
+      <c r="M37" s="97"/>
+      <c r="N37" s="122"/>
+      <c r="O37" s="125"/>
+      <c r="P37" s="128"/>
+      <c r="Q37" s="131"/>
       <c r="R37" s="31"/>
       <c r="S37" s="11"/>
       <c r="T37" s="23"/>
@@ -5149,37 +5483,53 @@
       <c r="AS37" s="4"/>
     </row>
     <row r="38" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="104" t="s">
+      <c r="A38" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="101" t="s">
+      <c r="B38" s="104" t="s">
         <v>111</v>
       </c>
       <c r="C38" s="98">
         <v>19</v>
       </c>
       <c r="D38" s="98" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E38" s="95" t="s">
         <v>109</v>
       </c>
       <c r="F38" s="95" t="s">
+        <v>151</v>
+      </c>
+      <c r="G38" s="95" t="s">
         <v>119</v>
       </c>
-      <c r="G38" s="95" t="s">
-        <v>121</v>
-      </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="24"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="31"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="23"/>
-      <c r="P38" s="24"/>
-      <c r="Q38" s="12"/>
+      <c r="H38" s="95" t="s">
+        <v>149</v>
+      </c>
+      <c r="I38" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J38" s="132"/>
+      <c r="K38" s="135">
+        <v>4</v>
+      </c>
+      <c r="L38" s="129">
+        <v>44859.599305555559</v>
+      </c>
+      <c r="M38" s="95" t="s">
+        <v>149</v>
+      </c>
+      <c r="N38" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="O38" s="132"/>
+      <c r="P38" s="135">
+        <v>6</v>
+      </c>
+      <c r="Q38" s="129">
+        <v>44859.607638888891</v>
+      </c>
       <c r="R38" s="31"/>
       <c r="S38" s="11"/>
       <c r="T38" s="23"/>
@@ -5193,23 +5543,23 @@
       <c r="AS38" s="4"/>
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A39" s="105"/>
-      <c r="B39" s="102"/>
+      <c r="A39" s="102"/>
+      <c r="B39" s="105"/>
       <c r="C39" s="99"/>
       <c r="D39" s="99"/>
       <c r="E39" s="96"/>
       <c r="F39" s="96"/>
       <c r="G39" s="96"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="24"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="31"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="24"/>
-      <c r="Q39" s="12"/>
+      <c r="H39" s="96"/>
+      <c r="I39" s="121"/>
+      <c r="J39" s="133"/>
+      <c r="K39" s="136"/>
+      <c r="L39" s="130"/>
+      <c r="M39" s="96"/>
+      <c r="N39" s="121"/>
+      <c r="O39" s="133"/>
+      <c r="P39" s="136"/>
+      <c r="Q39" s="130"/>
       <c r="R39" s="31"/>
       <c r="S39" s="11"/>
       <c r="T39" s="23"/>
@@ -5223,23 +5573,23 @@
       <c r="AS39" s="4"/>
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A40" s="105"/>
-      <c r="B40" s="102"/>
+      <c r="A40" s="102"/>
+      <c r="B40" s="105"/>
       <c r="C40" s="99"/>
       <c r="D40" s="99"/>
       <c r="E40" s="96"/>
       <c r="F40" s="96"/>
       <c r="G40" s="96"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="23"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="31"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="23"/>
-      <c r="P40" s="24"/>
-      <c r="Q40" s="12"/>
+      <c r="H40" s="96"/>
+      <c r="I40" s="121"/>
+      <c r="J40" s="133"/>
+      <c r="K40" s="136"/>
+      <c r="L40" s="130"/>
+      <c r="M40" s="96"/>
+      <c r="N40" s="121"/>
+      <c r="O40" s="133"/>
+      <c r="P40" s="136"/>
+      <c r="Q40" s="130"/>
       <c r="R40" s="31"/>
       <c r="S40" s="11"/>
       <c r="T40" s="23"/>
@@ -5253,23 +5603,23 @@
       <c r="AS40" s="4"/>
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A41" s="105"/>
-      <c r="B41" s="102"/>
+      <c r="A41" s="102"/>
+      <c r="B41" s="105"/>
       <c r="C41" s="99"/>
       <c r="D41" s="99"/>
       <c r="E41" s="96"/>
       <c r="F41" s="96"/>
       <c r="G41" s="96"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="24"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="24"/>
-      <c r="Q41" s="12"/>
+      <c r="H41" s="96"/>
+      <c r="I41" s="121"/>
+      <c r="J41" s="133"/>
+      <c r="K41" s="136"/>
+      <c r="L41" s="130"/>
+      <c r="M41" s="96"/>
+      <c r="N41" s="121"/>
+      <c r="O41" s="133"/>
+      <c r="P41" s="136"/>
+      <c r="Q41" s="130"/>
       <c r="R41" s="31"/>
       <c r="S41" s="11"/>
       <c r="T41" s="23"/>
@@ -5283,23 +5633,23 @@
       <c r="AS41" s="4"/>
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A42" s="105"/>
-      <c r="B42" s="102"/>
+      <c r="A42" s="102"/>
+      <c r="B42" s="105"/>
       <c r="C42" s="99"/>
       <c r="D42" s="99"/>
       <c r="E42" s="96"/>
       <c r="F42" s="96"/>
       <c r="G42" s="96"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="24"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="31"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="24"/>
-      <c r="Q42" s="12"/>
+      <c r="H42" s="96"/>
+      <c r="I42" s="121"/>
+      <c r="J42" s="133"/>
+      <c r="K42" s="136"/>
+      <c r="L42" s="130"/>
+      <c r="M42" s="96"/>
+      <c r="N42" s="121"/>
+      <c r="O42" s="133"/>
+      <c r="P42" s="136"/>
+      <c r="Q42" s="130"/>
       <c r="R42" s="31"/>
       <c r="S42" s="11"/>
       <c r="T42" s="23"/>
@@ -5313,23 +5663,23 @@
       <c r="AS42" s="4"/>
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A43" s="105"/>
-      <c r="B43" s="102"/>
+      <c r="A43" s="102"/>
+      <c r="B43" s="105"/>
       <c r="C43" s="99"/>
       <c r="D43" s="99"/>
       <c r="E43" s="96"/>
       <c r="F43" s="96"/>
       <c r="G43" s="96"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="24"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="24"/>
-      <c r="Q43" s="12"/>
+      <c r="H43" s="96"/>
+      <c r="I43" s="121"/>
+      <c r="J43" s="133"/>
+      <c r="K43" s="136"/>
+      <c r="L43" s="130"/>
+      <c r="M43" s="96"/>
+      <c r="N43" s="121"/>
+      <c r="O43" s="133"/>
+      <c r="P43" s="136"/>
+      <c r="Q43" s="130"/>
       <c r="R43" s="31"/>
       <c r="S43" s="11"/>
       <c r="T43" s="23"/>
@@ -5343,23 +5693,23 @@
       <c r="AS43" s="4"/>
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A44" s="105"/>
-      <c r="B44" s="102"/>
+      <c r="A44" s="102"/>
+      <c r="B44" s="105"/>
       <c r="C44" s="99"/>
       <c r="D44" s="99"/>
       <c r="E44" s="96"/>
       <c r="F44" s="96"/>
       <c r="G44" s="96"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="24"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="31"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="24"/>
-      <c r="Q44" s="12"/>
+      <c r="H44" s="96"/>
+      <c r="I44" s="121"/>
+      <c r="J44" s="133"/>
+      <c r="K44" s="136"/>
+      <c r="L44" s="130"/>
+      <c r="M44" s="96"/>
+      <c r="N44" s="121"/>
+      <c r="O44" s="133"/>
+      <c r="P44" s="136"/>
+      <c r="Q44" s="130"/>
       <c r="R44" s="31"/>
       <c r="S44" s="11"/>
       <c r="T44" s="23"/>
@@ -5373,23 +5723,23 @@
       <c r="AS44" s="4"/>
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A45" s="105"/>
-      <c r="B45" s="102"/>
+      <c r="A45" s="102"/>
+      <c r="B45" s="105"/>
       <c r="C45" s="99"/>
       <c r="D45" s="99"/>
       <c r="E45" s="96"/>
       <c r="F45" s="96"/>
       <c r="G45" s="96"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="31"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="23"/>
-      <c r="P45" s="24"/>
-      <c r="Q45" s="12"/>
+      <c r="H45" s="96"/>
+      <c r="I45" s="121"/>
+      <c r="J45" s="133"/>
+      <c r="K45" s="136"/>
+      <c r="L45" s="130"/>
+      <c r="M45" s="96"/>
+      <c r="N45" s="121"/>
+      <c r="O45" s="133"/>
+      <c r="P45" s="136"/>
+      <c r="Q45" s="130"/>
       <c r="R45" s="31"/>
       <c r="S45" s="11"/>
       <c r="T45" s="23"/>
@@ -5403,23 +5753,23 @@
       <c r="AS45" s="4"/>
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A46" s="105"/>
-      <c r="B46" s="102"/>
+      <c r="A46" s="102"/>
+      <c r="B46" s="105"/>
       <c r="C46" s="99"/>
       <c r="D46" s="99"/>
       <c r="E46" s="96"/>
       <c r="F46" s="96"/>
       <c r="G46" s="96"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="24"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="23"/>
-      <c r="P46" s="24"/>
-      <c r="Q46" s="12"/>
+      <c r="H46" s="96"/>
+      <c r="I46" s="121"/>
+      <c r="J46" s="133"/>
+      <c r="K46" s="136"/>
+      <c r="L46" s="130"/>
+      <c r="M46" s="96"/>
+      <c r="N46" s="121"/>
+      <c r="O46" s="133"/>
+      <c r="P46" s="136"/>
+      <c r="Q46" s="130"/>
       <c r="R46" s="31"/>
       <c r="S46" s="11"/>
       <c r="T46" s="23"/>
@@ -5433,23 +5783,23 @@
       <c r="AS46" s="4"/>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A47" s="105"/>
-      <c r="B47" s="102"/>
+      <c r="A47" s="102"/>
+      <c r="B47" s="105"/>
       <c r="C47" s="99"/>
       <c r="D47" s="99"/>
       <c r="E47" s="96"/>
       <c r="F47" s="96"/>
       <c r="G47" s="96"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="24"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="23"/>
-      <c r="P47" s="24"/>
-      <c r="Q47" s="12"/>
+      <c r="H47" s="96"/>
+      <c r="I47" s="121"/>
+      <c r="J47" s="133"/>
+      <c r="K47" s="136"/>
+      <c r="L47" s="130"/>
+      <c r="M47" s="96"/>
+      <c r="N47" s="121"/>
+      <c r="O47" s="133"/>
+      <c r="P47" s="136"/>
+      <c r="Q47" s="130"/>
       <c r="R47" s="31"/>
       <c r="S47" s="11"/>
       <c r="T47" s="23"/>
@@ -5463,23 +5813,23 @@
       <c r="AS47" s="4"/>
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A48" s="105"/>
-      <c r="B48" s="102"/>
+      <c r="A48" s="102"/>
+      <c r="B48" s="105"/>
       <c r="C48" s="99"/>
       <c r="D48" s="99"/>
       <c r="E48" s="96"/>
       <c r="F48" s="96"/>
       <c r="G48" s="96"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="24"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="31"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="23"/>
-      <c r="P48" s="24"/>
-      <c r="Q48" s="12"/>
+      <c r="H48" s="96"/>
+      <c r="I48" s="121"/>
+      <c r="J48" s="133"/>
+      <c r="K48" s="136"/>
+      <c r="L48" s="130"/>
+      <c r="M48" s="96"/>
+      <c r="N48" s="121"/>
+      <c r="O48" s="133"/>
+      <c r="P48" s="136"/>
+      <c r="Q48" s="130"/>
       <c r="R48" s="31"/>
       <c r="S48" s="11"/>
       <c r="T48" s="23"/>
@@ -5493,23 +5843,23 @@
       <c r="AS48" s="4"/>
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A49" s="105"/>
-      <c r="B49" s="102"/>
+      <c r="A49" s="102"/>
+      <c r="B49" s="105"/>
       <c r="C49" s="99"/>
       <c r="D49" s="99"/>
       <c r="E49" s="96"/>
       <c r="F49" s="96"/>
       <c r="G49" s="96"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="24"/>
-      <c r="L49" s="29"/>
-      <c r="M49" s="31"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="23"/>
-      <c r="P49" s="24"/>
-      <c r="Q49" s="12"/>
+      <c r="H49" s="96"/>
+      <c r="I49" s="121"/>
+      <c r="J49" s="133"/>
+      <c r="K49" s="136"/>
+      <c r="L49" s="130"/>
+      <c r="M49" s="96"/>
+      <c r="N49" s="121"/>
+      <c r="O49" s="133"/>
+      <c r="P49" s="136"/>
+      <c r="Q49" s="130"/>
       <c r="R49" s="31"/>
       <c r="S49" s="11"/>
       <c r="T49" s="23"/>
@@ -5523,23 +5873,23 @@
       <c r="AS49" s="4"/>
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A50" s="105"/>
-      <c r="B50" s="102"/>
+      <c r="A50" s="102"/>
+      <c r="B50" s="105"/>
       <c r="C50" s="99"/>
       <c r="D50" s="99"/>
       <c r="E50" s="96"/>
       <c r="F50" s="96"/>
       <c r="G50" s="96"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="24"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="31"/>
-      <c r="N50" s="11"/>
-      <c r="O50" s="23"/>
-      <c r="P50" s="24"/>
-      <c r="Q50" s="12"/>
+      <c r="H50" s="96"/>
+      <c r="I50" s="121"/>
+      <c r="J50" s="133"/>
+      <c r="K50" s="136"/>
+      <c r="L50" s="130"/>
+      <c r="M50" s="96"/>
+      <c r="N50" s="121"/>
+      <c r="O50" s="133"/>
+      <c r="P50" s="136"/>
+      <c r="Q50" s="130"/>
       <c r="R50" s="31"/>
       <c r="S50" s="11"/>
       <c r="T50" s="23"/>
@@ -5553,23 +5903,23 @@
       <c r="AS50" s="4"/>
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A51" s="105"/>
-      <c r="B51" s="102"/>
+      <c r="A51" s="102"/>
+      <c r="B51" s="105"/>
       <c r="C51" s="99"/>
       <c r="D51" s="99"/>
       <c r="E51" s="96"/>
       <c r="F51" s="96"/>
       <c r="G51" s="96"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="23"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="29"/>
-      <c r="M51" s="31"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="23"/>
-      <c r="P51" s="24"/>
-      <c r="Q51" s="12"/>
+      <c r="H51" s="96"/>
+      <c r="I51" s="121"/>
+      <c r="J51" s="133"/>
+      <c r="K51" s="136"/>
+      <c r="L51" s="130"/>
+      <c r="M51" s="96"/>
+      <c r="N51" s="121"/>
+      <c r="O51" s="133"/>
+      <c r="P51" s="136"/>
+      <c r="Q51" s="130"/>
       <c r="R51" s="31"/>
       <c r="S51" s="11"/>
       <c r="T51" s="23"/>
@@ -5583,23 +5933,23 @@
       <c r="AS51" s="4"/>
     </row>
     <row r="52" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A52" s="105"/>
-      <c r="B52" s="102"/>
+      <c r="A52" s="102"/>
+      <c r="B52" s="105"/>
       <c r="C52" s="99"/>
       <c r="D52" s="99"/>
       <c r="E52" s="96"/>
       <c r="F52" s="96"/>
       <c r="G52" s="96"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="23"/>
-      <c r="K52" s="24"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="31"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="23"/>
-      <c r="P52" s="24"/>
-      <c r="Q52" s="12"/>
+      <c r="H52" s="96"/>
+      <c r="I52" s="121"/>
+      <c r="J52" s="133"/>
+      <c r="K52" s="136"/>
+      <c r="L52" s="130"/>
+      <c r="M52" s="96"/>
+      <c r="N52" s="121"/>
+      <c r="O52" s="133"/>
+      <c r="P52" s="136"/>
+      <c r="Q52" s="130"/>
       <c r="R52" s="31"/>
       <c r="S52" s="11"/>
       <c r="T52" s="23"/>
@@ -5613,23 +5963,23 @@
       <c r="AS52" s="4"/>
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A53" s="105"/>
-      <c r="B53" s="102"/>
+      <c r="A53" s="102"/>
+      <c r="B53" s="105"/>
       <c r="C53" s="99"/>
       <c r="D53" s="99"/>
       <c r="E53" s="96"/>
       <c r="F53" s="96"/>
       <c r="G53" s="96"/>
-      <c r="H53" s="22"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="23"/>
-      <c r="K53" s="24"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="31"/>
-      <c r="N53" s="11"/>
-      <c r="O53" s="23"/>
-      <c r="P53" s="24"/>
-      <c r="Q53" s="12"/>
+      <c r="H53" s="96"/>
+      <c r="I53" s="121"/>
+      <c r="J53" s="133"/>
+      <c r="K53" s="136"/>
+      <c r="L53" s="130"/>
+      <c r="M53" s="96"/>
+      <c r="N53" s="121"/>
+      <c r="O53" s="133"/>
+      <c r="P53" s="136"/>
+      <c r="Q53" s="130"/>
       <c r="R53" s="31"/>
       <c r="S53" s="11"/>
       <c r="T53" s="23"/>
@@ -5643,23 +5993,23 @@
       <c r="AS53" s="4"/>
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A54" s="105"/>
-      <c r="B54" s="102"/>
+      <c r="A54" s="102"/>
+      <c r="B54" s="105"/>
       <c r="C54" s="99"/>
       <c r="D54" s="99"/>
       <c r="E54" s="96"/>
       <c r="F54" s="96"/>
       <c r="G54" s="96"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="23"/>
-      <c r="K54" s="24"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="31"/>
-      <c r="N54" s="11"/>
-      <c r="O54" s="23"/>
-      <c r="P54" s="24"/>
-      <c r="Q54" s="12"/>
+      <c r="H54" s="96"/>
+      <c r="I54" s="121"/>
+      <c r="J54" s="133"/>
+      <c r="K54" s="136"/>
+      <c r="L54" s="130"/>
+      <c r="M54" s="96"/>
+      <c r="N54" s="121"/>
+      <c r="O54" s="133"/>
+      <c r="P54" s="136"/>
+      <c r="Q54" s="130"/>
       <c r="R54" s="31"/>
       <c r="S54" s="11"/>
       <c r="T54" s="23"/>
@@ -5673,23 +6023,23 @@
       <c r="AS54" s="4"/>
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A55" s="105"/>
-      <c r="B55" s="102"/>
+      <c r="A55" s="102"/>
+      <c r="B55" s="105"/>
       <c r="C55" s="99"/>
       <c r="D55" s="99"/>
       <c r="E55" s="96"/>
       <c r="F55" s="96"/>
       <c r="G55" s="96"/>
-      <c r="H55" s="22"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="23"/>
-      <c r="K55" s="24"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="31"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="23"/>
-      <c r="P55" s="24"/>
-      <c r="Q55" s="12"/>
+      <c r="H55" s="96"/>
+      <c r="I55" s="121"/>
+      <c r="J55" s="133"/>
+      <c r="K55" s="136"/>
+      <c r="L55" s="130"/>
+      <c r="M55" s="96"/>
+      <c r="N55" s="121"/>
+      <c r="O55" s="133"/>
+      <c r="P55" s="136"/>
+      <c r="Q55" s="130"/>
       <c r="R55" s="31"/>
       <c r="S55" s="11"/>
       <c r="T55" s="23"/>
@@ -5703,23 +6053,23 @@
       <c r="AS55" s="4"/>
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A56" s="105"/>
-      <c r="B56" s="102"/>
+      <c r="A56" s="102"/>
+      <c r="B56" s="105"/>
       <c r="C56" s="99"/>
       <c r="D56" s="99"/>
       <c r="E56" s="96"/>
       <c r="F56" s="96"/>
       <c r="G56" s="96"/>
-      <c r="H56" s="22"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="23"/>
-      <c r="K56" s="24"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="31"/>
-      <c r="N56" s="11"/>
-      <c r="O56" s="23"/>
-      <c r="P56" s="24"/>
-      <c r="Q56" s="12"/>
+      <c r="H56" s="96"/>
+      <c r="I56" s="121"/>
+      <c r="J56" s="133"/>
+      <c r="K56" s="136"/>
+      <c r="L56" s="130"/>
+      <c r="M56" s="96"/>
+      <c r="N56" s="121"/>
+      <c r="O56" s="133"/>
+      <c r="P56" s="136"/>
+      <c r="Q56" s="130"/>
       <c r="R56" s="31"/>
       <c r="S56" s="11"/>
       <c r="T56" s="23"/>
@@ -5733,23 +6083,23 @@
       <c r="AS56" s="4"/>
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A57" s="105"/>
-      <c r="B57" s="102"/>
+      <c r="A57" s="102"/>
+      <c r="B57" s="105"/>
       <c r="C57" s="99"/>
       <c r="D57" s="99"/>
       <c r="E57" s="96"/>
       <c r="F57" s="96"/>
       <c r="G57" s="96"/>
-      <c r="H57" s="22"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="23"/>
-      <c r="K57" s="24"/>
-      <c r="L57" s="29"/>
-      <c r="M57" s="31"/>
-      <c r="N57" s="11"/>
-      <c r="O57" s="23"/>
-      <c r="P57" s="24"/>
-      <c r="Q57" s="12"/>
+      <c r="H57" s="96"/>
+      <c r="I57" s="121"/>
+      <c r="J57" s="133"/>
+      <c r="K57" s="136"/>
+      <c r="L57" s="130"/>
+      <c r="M57" s="96"/>
+      <c r="N57" s="121"/>
+      <c r="O57" s="133"/>
+      <c r="P57" s="136"/>
+      <c r="Q57" s="130"/>
       <c r="R57" s="31"/>
       <c r="S57" s="11"/>
       <c r="T57" s="23"/>
@@ -5763,23 +6113,23 @@
       <c r="AS57" s="4"/>
     </row>
     <row r="58" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A58" s="105"/>
-      <c r="B58" s="102"/>
+      <c r="A58" s="102"/>
+      <c r="B58" s="105"/>
       <c r="C58" s="99"/>
       <c r="D58" s="99"/>
       <c r="E58" s="96"/>
       <c r="F58" s="96"/>
       <c r="G58" s="96"/>
-      <c r="H58" s="22"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="23"/>
-      <c r="K58" s="24"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="31"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="23"/>
-      <c r="P58" s="24"/>
-      <c r="Q58" s="12"/>
+      <c r="H58" s="96"/>
+      <c r="I58" s="121"/>
+      <c r="J58" s="133"/>
+      <c r="K58" s="136"/>
+      <c r="L58" s="130"/>
+      <c r="M58" s="96"/>
+      <c r="N58" s="121"/>
+      <c r="O58" s="133"/>
+      <c r="P58" s="136"/>
+      <c r="Q58" s="130"/>
       <c r="R58" s="31"/>
       <c r="S58" s="11"/>
       <c r="T58" s="23"/>
@@ -5793,23 +6143,23 @@
       <c r="AS58" s="4"/>
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A59" s="106"/>
-      <c r="B59" s="103"/>
+      <c r="A59" s="103"/>
+      <c r="B59" s="106"/>
       <c r="C59" s="100"/>
       <c r="D59" s="100"/>
       <c r="E59" s="97"/>
       <c r="F59" s="97"/>
       <c r="G59" s="97"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="24"/>
-      <c r="L59" s="29"/>
-      <c r="M59" s="31"/>
-      <c r="N59" s="11"/>
-      <c r="O59" s="23"/>
-      <c r="P59" s="24"/>
-      <c r="Q59" s="12"/>
+      <c r="H59" s="97"/>
+      <c r="I59" s="122"/>
+      <c r="J59" s="134"/>
+      <c r="K59" s="137"/>
+      <c r="L59" s="131"/>
+      <c r="M59" s="97"/>
+      <c r="N59" s="122"/>
+      <c r="O59" s="134"/>
+      <c r="P59" s="137"/>
+      <c r="Q59" s="131"/>
       <c r="R59" s="31"/>
       <c r="S59" s="11"/>
       <c r="T59" s="23"/>
@@ -5823,32 +6173,40 @@
       <c r="AS59" s="4"/>
     </row>
     <row r="60" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A60" s="104" t="s">
+      <c r="A60" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="101" t="s">
+      <c r="B60" s="104" t="s">
         <v>111</v>
       </c>
       <c r="C60" s="98">
         <v>19</v>
       </c>
       <c r="D60" s="98" t="s">
+        <v>120</v>
+      </c>
+      <c r="E60" s="95" t="s">
+        <v>121</v>
+      </c>
+      <c r="F60" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="E60" s="95" t="s">
+      <c r="G60" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="F60" s="95" t="s">
-        <v>124</v>
-      </c>
-      <c r="G60" s="95" t="s">
-        <v>125</v>
-      </c>
-      <c r="H60" s="22"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="23"/>
-      <c r="K60" s="24"/>
-      <c r="L60" s="29"/>
+      <c r="H60" s="95" t="s">
+        <v>148</v>
+      </c>
+      <c r="I60" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J60" s="95"/>
+      <c r="K60" s="95">
+        <v>7</v>
+      </c>
+      <c r="L60" s="129">
+        <v>44859.611111111109</v>
+      </c>
       <c r="M60" s="31"/>
       <c r="N60" s="11"/>
       <c r="O60" s="23"/>
@@ -5867,18 +6225,18 @@
       <c r="AS60" s="4"/>
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A61" s="105"/>
-      <c r="B61" s="102"/>
+      <c r="A61" s="102"/>
+      <c r="B61" s="105"/>
       <c r="C61" s="99"/>
       <c r="D61" s="99"/>
       <c r="E61" s="96"/>
       <c r="F61" s="96"/>
       <c r="G61" s="96"/>
-      <c r="H61" s="22"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="23"/>
-      <c r="K61" s="24"/>
-      <c r="L61" s="29"/>
+      <c r="H61" s="96"/>
+      <c r="I61" s="121"/>
+      <c r="J61" s="96"/>
+      <c r="K61" s="96"/>
+      <c r="L61" s="130"/>
       <c r="M61" s="31"/>
       <c r="N61" s="11"/>
       <c r="O61" s="23"/>
@@ -5897,18 +6255,18 @@
       <c r="AS61" s="4"/>
     </row>
     <row r="62" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A62" s="105"/>
-      <c r="B62" s="102"/>
+      <c r="A62" s="102"/>
+      <c r="B62" s="105"/>
       <c r="C62" s="99"/>
       <c r="D62" s="99"/>
       <c r="E62" s="96"/>
       <c r="F62" s="96"/>
       <c r="G62" s="96"/>
-      <c r="H62" s="22"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="23"/>
-      <c r="K62" s="24"/>
-      <c r="L62" s="29"/>
+      <c r="H62" s="96"/>
+      <c r="I62" s="121"/>
+      <c r="J62" s="96"/>
+      <c r="K62" s="96"/>
+      <c r="L62" s="130"/>
       <c r="M62" s="31"/>
       <c r="N62" s="11"/>
       <c r="O62" s="23"/>
@@ -5927,18 +6285,18 @@
       <c r="AS62" s="4"/>
     </row>
     <row r="63" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A63" s="105"/>
-      <c r="B63" s="102"/>
+      <c r="A63" s="102"/>
+      <c r="B63" s="105"/>
       <c r="C63" s="99"/>
       <c r="D63" s="99"/>
       <c r="E63" s="96"/>
       <c r="F63" s="96"/>
       <c r="G63" s="96"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="23"/>
-      <c r="K63" s="24"/>
-      <c r="L63" s="29"/>
+      <c r="H63" s="96"/>
+      <c r="I63" s="121"/>
+      <c r="J63" s="96"/>
+      <c r="K63" s="96"/>
+      <c r="L63" s="130"/>
       <c r="M63" s="31"/>
       <c r="N63" s="11"/>
       <c r="O63" s="23"/>
@@ -5957,18 +6315,18 @@
       <c r="AS63" s="4"/>
     </row>
     <row r="64" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A64" s="105"/>
-      <c r="B64" s="102"/>
+      <c r="A64" s="102"/>
+      <c r="B64" s="105"/>
       <c r="C64" s="99"/>
       <c r="D64" s="99"/>
       <c r="E64" s="96"/>
       <c r="F64" s="96"/>
       <c r="G64" s="96"/>
-      <c r="H64" s="22"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="23"/>
-      <c r="K64" s="24"/>
-      <c r="L64" s="29"/>
+      <c r="H64" s="96"/>
+      <c r="I64" s="121"/>
+      <c r="J64" s="96"/>
+      <c r="K64" s="96"/>
+      <c r="L64" s="130"/>
       <c r="M64" s="31"/>
       <c r="N64" s="11"/>
       <c r="O64" s="23"/>
@@ -5987,18 +6345,18 @@
       <c r="AS64" s="4"/>
     </row>
     <row r="65" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A65" s="105"/>
-      <c r="B65" s="102"/>
+      <c r="A65" s="102"/>
+      <c r="B65" s="105"/>
       <c r="C65" s="99"/>
       <c r="D65" s="99"/>
       <c r="E65" s="96"/>
       <c r="F65" s="96"/>
       <c r="G65" s="96"/>
-      <c r="H65" s="22"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="23"/>
-      <c r="K65" s="24"/>
-      <c r="L65" s="29"/>
+      <c r="H65" s="96"/>
+      <c r="I65" s="121"/>
+      <c r="J65" s="96"/>
+      <c r="K65" s="96"/>
+      <c r="L65" s="130"/>
       <c r="M65" s="31"/>
       <c r="N65" s="11"/>
       <c r="O65" s="23"/>
@@ -6017,18 +6375,18 @@
       <c r="AS65" s="4"/>
     </row>
     <row r="66" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A66" s="105"/>
-      <c r="B66" s="102"/>
+      <c r="A66" s="102"/>
+      <c r="B66" s="105"/>
       <c r="C66" s="99"/>
       <c r="D66" s="99"/>
       <c r="E66" s="96"/>
       <c r="F66" s="96"/>
       <c r="G66" s="96"/>
-      <c r="H66" s="22"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="23"/>
-      <c r="K66" s="24"/>
-      <c r="L66" s="29"/>
+      <c r="H66" s="96"/>
+      <c r="I66" s="121"/>
+      <c r="J66" s="96"/>
+      <c r="K66" s="96"/>
+      <c r="L66" s="130"/>
       <c r="M66" s="31"/>
       <c r="N66" s="11"/>
       <c r="O66" s="23"/>
@@ -6047,18 +6405,18 @@
       <c r="AS66" s="4"/>
     </row>
     <row r="67" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A67" s="105"/>
-      <c r="B67" s="102"/>
+      <c r="A67" s="102"/>
+      <c r="B67" s="105"/>
       <c r="C67" s="99"/>
       <c r="D67" s="99"/>
       <c r="E67" s="96"/>
       <c r="F67" s="96"/>
       <c r="G67" s="96"/>
-      <c r="H67" s="22"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="24"/>
-      <c r="L67" s="29"/>
+      <c r="H67" s="96"/>
+      <c r="I67" s="121"/>
+      <c r="J67" s="96"/>
+      <c r="K67" s="96"/>
+      <c r="L67" s="130"/>
       <c r="M67" s="31"/>
       <c r="N67" s="11"/>
       <c r="O67" s="23"/>
@@ -6077,18 +6435,18 @@
       <c r="AS67" s="4"/>
     </row>
     <row r="68" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A68" s="105"/>
-      <c r="B68" s="102"/>
+      <c r="A68" s="102"/>
+      <c r="B68" s="105"/>
       <c r="C68" s="99"/>
       <c r="D68" s="99"/>
       <c r="E68" s="96"/>
       <c r="F68" s="96"/>
       <c r="G68" s="96"/>
-      <c r="H68" s="22"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="23"/>
-      <c r="K68" s="24"/>
-      <c r="L68" s="29"/>
+      <c r="H68" s="96"/>
+      <c r="I68" s="121"/>
+      <c r="J68" s="96"/>
+      <c r="K68" s="96"/>
+      <c r="L68" s="130"/>
       <c r="M68" s="31"/>
       <c r="N68" s="11"/>
       <c r="O68" s="23"/>
@@ -6107,18 +6465,18 @@
       <c r="AS68" s="4"/>
     </row>
     <row r="69" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A69" s="105"/>
-      <c r="B69" s="102"/>
+      <c r="A69" s="102"/>
+      <c r="B69" s="105"/>
       <c r="C69" s="99"/>
       <c r="D69" s="99"/>
       <c r="E69" s="96"/>
       <c r="F69" s="96"/>
       <c r="G69" s="96"/>
-      <c r="H69" s="22"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="23"/>
-      <c r="K69" s="24"/>
-      <c r="L69" s="29"/>
+      <c r="H69" s="96"/>
+      <c r="I69" s="121"/>
+      <c r="J69" s="96"/>
+      <c r="K69" s="96"/>
+      <c r="L69" s="130"/>
       <c r="M69" s="31"/>
       <c r="N69" s="11"/>
       <c r="O69" s="23"/>
@@ -6137,18 +6495,18 @@
       <c r="AS69" s="4"/>
     </row>
     <row r="70" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A70" s="105"/>
-      <c r="B70" s="102"/>
+      <c r="A70" s="102"/>
+      <c r="B70" s="105"/>
       <c r="C70" s="99"/>
       <c r="D70" s="99"/>
       <c r="E70" s="96"/>
       <c r="F70" s="96"/>
       <c r="G70" s="96"/>
-      <c r="H70" s="22"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="23"/>
-      <c r="K70" s="24"/>
-      <c r="L70" s="29"/>
+      <c r="H70" s="96"/>
+      <c r="I70" s="121"/>
+      <c r="J70" s="96"/>
+      <c r="K70" s="96"/>
+      <c r="L70" s="130"/>
       <c r="M70" s="31"/>
       <c r="N70" s="11"/>
       <c r="O70" s="23"/>
@@ -6167,18 +6525,18 @@
       <c r="AS70" s="4"/>
     </row>
     <row r="71" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A71" s="105"/>
-      <c r="B71" s="102"/>
+      <c r="A71" s="102"/>
+      <c r="B71" s="105"/>
       <c r="C71" s="99"/>
       <c r="D71" s="99"/>
       <c r="E71" s="96"/>
       <c r="F71" s="96"/>
       <c r="G71" s="96"/>
-      <c r="H71" s="22"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="23"/>
-      <c r="K71" s="24"/>
-      <c r="L71" s="29"/>
+      <c r="H71" s="96"/>
+      <c r="I71" s="121"/>
+      <c r="J71" s="96"/>
+      <c r="K71" s="96"/>
+      <c r="L71" s="130"/>
       <c r="M71" s="31"/>
       <c r="N71" s="11"/>
       <c r="O71" s="23"/>
@@ -6197,18 +6555,18 @@
       <c r="AS71" s="4"/>
     </row>
     <row r="72" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A72" s="105"/>
-      <c r="B72" s="102"/>
+      <c r="A72" s="102"/>
+      <c r="B72" s="105"/>
       <c r="C72" s="99"/>
       <c r="D72" s="99"/>
       <c r="E72" s="96"/>
       <c r="F72" s="96"/>
       <c r="G72" s="96"/>
-      <c r="H72" s="22"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="23"/>
-      <c r="K72" s="24"/>
-      <c r="L72" s="29"/>
+      <c r="H72" s="96"/>
+      <c r="I72" s="121"/>
+      <c r="J72" s="96"/>
+      <c r="K72" s="96"/>
+      <c r="L72" s="130"/>
       <c r="M72" s="31"/>
       <c r="N72" s="11"/>
       <c r="O72" s="23"/>
@@ -6227,18 +6585,18 @@
       <c r="AS72" s="4"/>
     </row>
     <row r="73" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A73" s="106"/>
-      <c r="B73" s="103"/>
+      <c r="A73" s="103"/>
+      <c r="B73" s="106"/>
       <c r="C73" s="100"/>
       <c r="D73" s="100"/>
       <c r="E73" s="97"/>
       <c r="F73" s="97"/>
       <c r="G73" s="97"/>
-      <c r="H73" s="22"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="23"/>
-      <c r="K73" s="24"/>
-      <c r="L73" s="29"/>
+      <c r="H73" s="97"/>
+      <c r="I73" s="122"/>
+      <c r="J73" s="97"/>
+      <c r="K73" s="97"/>
+      <c r="L73" s="131"/>
       <c r="M73" s="31"/>
       <c r="N73" s="11"/>
       <c r="O73" s="23"/>
@@ -6256,9 +6614,342 @@
       <c r="AR73" s="4"/>
       <c r="AS73" s="4"/>
     </row>
+    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A74" s="101" t="s">
+        <v>160</v>
+      </c>
+      <c r="B74" s="104" t="s">
+        <v>111</v>
+      </c>
+      <c r="C74" s="98">
+        <v>18</v>
+      </c>
+      <c r="D74" s="98" t="s">
+        <v>150</v>
+      </c>
+      <c r="E74" s="95" t="s">
+        <v>121</v>
+      </c>
+      <c r="F74" s="95" t="s">
+        <v>152</v>
+      </c>
+      <c r="G74" s="95" t="s">
+        <v>153</v>
+      </c>
+      <c r="H74" s="95" t="s">
+        <v>154</v>
+      </c>
+      <c r="I74" s="138" t="s">
+        <v>132</v>
+      </c>
+      <c r="J74" s="95"/>
+      <c r="K74" s="140">
+        <v>5</v>
+      </c>
+      <c r="L74" s="129">
+        <v>44859.600694444445</v>
+      </c>
+      <c r="M74" s="95" t="s">
+        <v>154</v>
+      </c>
+      <c r="N74" s="138" t="s">
+        <v>132</v>
+      </c>
+      <c r="O74" s="95"/>
+      <c r="P74" s="140">
+        <v>5</v>
+      </c>
+      <c r="Q74" s="129">
+        <v>44859.600694444445</v>
+      </c>
+    </row>
+    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A75" s="102"/>
+      <c r="B75" s="105"/>
+      <c r="C75" s="99"/>
+      <c r="D75" s="99"/>
+      <c r="E75" s="96"/>
+      <c r="F75" s="96"/>
+      <c r="G75" s="96"/>
+      <c r="H75" s="96"/>
+      <c r="I75" s="139"/>
+      <c r="J75" s="96"/>
+      <c r="K75" s="141"/>
+      <c r="L75" s="130"/>
+      <c r="M75" s="96"/>
+      <c r="N75" s="139"/>
+      <c r="O75" s="96"/>
+      <c r="P75" s="141"/>
+      <c r="Q75" s="130"/>
+    </row>
+    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A76" s="102"/>
+      <c r="B76" s="105"/>
+      <c r="C76" s="99"/>
+      <c r="D76" s="99"/>
+      <c r="E76" s="96"/>
+      <c r="F76" s="96"/>
+      <c r="G76" s="96"/>
+      <c r="H76" s="96"/>
+      <c r="I76" s="139"/>
+      <c r="J76" s="96"/>
+      <c r="K76" s="141"/>
+      <c r="L76" s="130"/>
+      <c r="M76" s="96"/>
+      <c r="N76" s="139"/>
+      <c r="O76" s="96"/>
+      <c r="P76" s="141"/>
+      <c r="Q76" s="130"/>
+    </row>
+    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A77" s="102"/>
+      <c r="B77" s="105"/>
+      <c r="C77" s="99"/>
+      <c r="D77" s="99"/>
+      <c r="E77" s="96"/>
+      <c r="F77" s="96"/>
+      <c r="G77" s="96"/>
+      <c r="H77" s="96"/>
+      <c r="I77" s="139"/>
+      <c r="J77" s="96"/>
+      <c r="K77" s="141"/>
+      <c r="L77" s="130"/>
+      <c r="M77" s="96"/>
+      <c r="N77" s="139"/>
+      <c r="O77" s="96"/>
+      <c r="P77" s="141"/>
+      <c r="Q77" s="130"/>
+    </row>
+    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A78" s="102"/>
+      <c r="B78" s="105"/>
+      <c r="C78" s="99"/>
+      <c r="D78" s="99"/>
+      <c r="E78" s="96"/>
+      <c r="F78" s="96"/>
+      <c r="G78" s="96"/>
+      <c r="H78" s="96"/>
+      <c r="I78" s="139"/>
+      <c r="J78" s="96"/>
+      <c r="K78" s="141"/>
+      <c r="L78" s="130"/>
+      <c r="M78" s="96"/>
+      <c r="N78" s="139"/>
+      <c r="O78" s="96"/>
+      <c r="P78" s="141"/>
+      <c r="Q78" s="130"/>
+    </row>
+    <row r="79" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A79" s="102"/>
+      <c r="B79" s="105"/>
+      <c r="C79" s="99"/>
+      <c r="D79" s="99"/>
+      <c r="E79" s="96"/>
+      <c r="F79" s="96"/>
+      <c r="G79" s="96"/>
+      <c r="H79" s="96"/>
+      <c r="I79" s="139"/>
+      <c r="J79" s="96"/>
+      <c r="K79" s="141"/>
+      <c r="L79" s="130"/>
+      <c r="M79" s="96"/>
+      <c r="N79" s="139"/>
+      <c r="O79" s="96"/>
+      <c r="P79" s="141"/>
+      <c r="Q79" s="130"/>
+    </row>
+    <row r="80" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A80" s="102"/>
+      <c r="B80" s="105"/>
+      <c r="C80" s="99"/>
+      <c r="D80" s="99"/>
+      <c r="E80" s="96"/>
+      <c r="F80" s="96"/>
+      <c r="G80" s="96"/>
+      <c r="H80" s="96"/>
+      <c r="I80" s="139"/>
+      <c r="J80" s="96"/>
+      <c r="K80" s="141"/>
+      <c r="L80" s="130"/>
+      <c r="M80" s="96"/>
+      <c r="N80" s="139"/>
+      <c r="O80" s="96"/>
+      <c r="P80" s="141"/>
+      <c r="Q80" s="130"/>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A81" s="102"/>
+      <c r="B81" s="105"/>
+      <c r="C81" s="99"/>
+      <c r="D81" s="99"/>
+      <c r="E81" s="96"/>
+      <c r="F81" s="96"/>
+      <c r="G81" s="96"/>
+      <c r="H81" s="96"/>
+      <c r="I81" s="139"/>
+      <c r="J81" s="96"/>
+      <c r="K81" s="141"/>
+      <c r="L81" s="130"/>
+      <c r="M81" s="96"/>
+      <c r="N81" s="139"/>
+      <c r="O81" s="96"/>
+      <c r="P81" s="141"/>
+      <c r="Q81" s="130"/>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A82" s="102"/>
+      <c r="B82" s="105"/>
+      <c r="C82" s="99"/>
+      <c r="D82" s="99"/>
+      <c r="E82" s="96"/>
+      <c r="F82" s="96"/>
+      <c r="G82" s="96"/>
+      <c r="H82" s="96"/>
+      <c r="I82" s="139"/>
+      <c r="J82" s="96"/>
+      <c r="K82" s="141"/>
+      <c r="L82" s="130"/>
+      <c r="M82" s="96"/>
+      <c r="N82" s="139"/>
+      <c r="O82" s="96"/>
+      <c r="P82" s="141"/>
+      <c r="Q82" s="130"/>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A83" s="102"/>
+      <c r="B83" s="105"/>
+      <c r="C83" s="99"/>
+      <c r="D83" s="99"/>
+      <c r="E83" s="96"/>
+      <c r="F83" s="96"/>
+      <c r="G83" s="96"/>
+      <c r="H83" s="96"/>
+      <c r="I83" s="139"/>
+      <c r="J83" s="96"/>
+      <c r="K83" s="141"/>
+      <c r="L83" s="130"/>
+      <c r="M83" s="96"/>
+      <c r="N83" s="139"/>
+      <c r="O83" s="96"/>
+      <c r="P83" s="141"/>
+      <c r="Q83" s="130"/>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" s="102"/>
+      <c r="B84" s="105"/>
+      <c r="C84" s="99"/>
+      <c r="D84" s="99"/>
+      <c r="E84" s="96"/>
+      <c r="F84" s="96"/>
+      <c r="G84" s="96"/>
+      <c r="H84" s="96"/>
+      <c r="I84" s="139"/>
+      <c r="J84" s="96"/>
+      <c r="K84" s="141"/>
+      <c r="L84" s="130"/>
+      <c r="M84" s="96"/>
+      <c r="N84" s="139"/>
+      <c r="O84" s="96"/>
+      <c r="P84" s="141"/>
+      <c r="Q84" s="130"/>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A85" s="102"/>
+      <c r="B85" s="105"/>
+      <c r="C85" s="99"/>
+      <c r="D85" s="99"/>
+      <c r="E85" s="96"/>
+      <c r="F85" s="96"/>
+      <c r="G85" s="96"/>
+      <c r="H85" s="96"/>
+      <c r="I85" s="139"/>
+      <c r="J85" s="96"/>
+      <c r="K85" s="141"/>
+      <c r="L85" s="130"/>
+      <c r="M85" s="96"/>
+      <c r="N85" s="139"/>
+      <c r="O85" s="96"/>
+      <c r="P85" s="141"/>
+      <c r="Q85" s="130"/>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A86" s="102"/>
+      <c r="B86" s="105"/>
+      <c r="C86" s="99"/>
+      <c r="D86" s="99"/>
+      <c r="E86" s="96"/>
+      <c r="F86" s="96"/>
+      <c r="G86" s="96"/>
+      <c r="H86" s="96"/>
+      <c r="I86" s="139"/>
+      <c r="J86" s="96"/>
+      <c r="K86" s="141"/>
+      <c r="L86" s="130"/>
+      <c r="M86" s="96"/>
+      <c r="N86" s="139"/>
+      <c r="O86" s="96"/>
+      <c r="P86" s="141"/>
+      <c r="Q86" s="130"/>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A87" s="103"/>
+      <c r="B87" s="106"/>
+      <c r="C87" s="100"/>
+      <c r="D87" s="100"/>
+      <c r="E87" s="97"/>
+      <c r="F87" s="97"/>
+      <c r="G87" s="97"/>
+      <c r="H87" s="97"/>
+      <c r="I87" s="139"/>
+      <c r="J87" s="97"/>
+      <c r="K87" s="142"/>
+      <c r="L87" s="131"/>
+      <c r="M87" s="97"/>
+      <c r="N87" s="139"/>
+      <c r="O87" s="97"/>
+      <c r="P87" s="142"/>
+      <c r="Q87" s="131"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A9:AS2331"/>
-  <mergeCells count="28">
+  <autoFilter ref="A9:AS2331" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <mergeCells count="70">
+    <mergeCell ref="M74:M87"/>
+    <mergeCell ref="N74:N87"/>
+    <mergeCell ref="O74:O87"/>
+    <mergeCell ref="P74:P87"/>
+    <mergeCell ref="Q74:Q87"/>
+    <mergeCell ref="F74:F87"/>
+    <mergeCell ref="G74:G87"/>
+    <mergeCell ref="H74:H87"/>
+    <mergeCell ref="I74:I87"/>
+    <mergeCell ref="J74:J87"/>
+    <mergeCell ref="A74:A87"/>
+    <mergeCell ref="B74:B87"/>
+    <mergeCell ref="C74:C87"/>
+    <mergeCell ref="D74:D87"/>
+    <mergeCell ref="E74:E87"/>
+    <mergeCell ref="M15:M37"/>
+    <mergeCell ref="N15:N37"/>
+    <mergeCell ref="O15:O37"/>
+    <mergeCell ref="P15:P37"/>
+    <mergeCell ref="Q15:Q37"/>
+    <mergeCell ref="M38:M59"/>
+    <mergeCell ref="N38:N59"/>
+    <mergeCell ref="O38:O59"/>
+    <mergeCell ref="P38:P59"/>
+    <mergeCell ref="Q38:Q59"/>
+    <mergeCell ref="L38:L59"/>
+    <mergeCell ref="H60:H73"/>
+    <mergeCell ref="I60:I73"/>
+    <mergeCell ref="J60:J73"/>
+    <mergeCell ref="K60:K73"/>
+    <mergeCell ref="L60:L73"/>
+    <mergeCell ref="K74:K87"/>
+    <mergeCell ref="L74:L87"/>
+    <mergeCell ref="H38:H59"/>
+    <mergeCell ref="I38:I59"/>
+    <mergeCell ref="J38:J59"/>
+    <mergeCell ref="K38:K59"/>
     <mergeCell ref="M8:Q8"/>
     <mergeCell ref="R8:V8"/>
     <mergeCell ref="A5:B5"/>
@@ -6273,22 +6964,27 @@
     <mergeCell ref="C15:C37"/>
     <mergeCell ref="B15:B37"/>
     <mergeCell ref="A15:A37"/>
+    <mergeCell ref="H15:H37"/>
+    <mergeCell ref="I15:I37"/>
+    <mergeCell ref="J15:J37"/>
+    <mergeCell ref="K15:K37"/>
+    <mergeCell ref="L15:L37"/>
     <mergeCell ref="D38:D59"/>
     <mergeCell ref="C38:C59"/>
     <mergeCell ref="A38:A59"/>
     <mergeCell ref="B38:B59"/>
     <mergeCell ref="B60:B73"/>
     <mergeCell ref="A60:A73"/>
+    <mergeCell ref="D60:D73"/>
+    <mergeCell ref="C60:C73"/>
     <mergeCell ref="F38:F59"/>
     <mergeCell ref="G38:G59"/>
     <mergeCell ref="E38:E59"/>
     <mergeCell ref="F60:F73"/>
     <mergeCell ref="G60:G73"/>
     <mergeCell ref="E60:E73"/>
-    <mergeCell ref="D60:D73"/>
-    <mergeCell ref="C60:C73"/>
   </mergeCells>
-  <conditionalFormatting sqref="J623:J747 J749 J751 J753 J755 J757 J759 J761 J763 J765:J771 J919:J1042 J1044:J1181 J1186:J1200 J1205:J1209 J1214:J1263 J1267:J1291 J1293:J1385 J1389:J1413 J1415:J1474 J1476:J1562 J1601:J1622 J1759:J1760 J1763:J1790 J1918:J1959 J1962:J1964 J1967 J1969:J1971 J1974:J2011 J2014:J2054 J2057:J2079 J2082:J2085 J2088 J2090:J2092 J2095:J2136 J2332:J65044 J9:J10 O623:O747 O749 O751 O753 O755 O757 O759 O761 O763 O765:O771 O919:O1042 O1044:O1181 O1186:O1200 O1205:O1209 O1214:O1263 O1267:O1291 O1293:O1385 O1389:O1413 O1415:O1474 O1476:O1562 O1601:O1622 O1759:O1760 O1763:O1790 O1918:O1959 O1962:O1964 O1967 O1969:O1971 O1974:O2011 O2014:O2054 O2057:O2079 O2082:O2085 O2088 O2090:O2092 O2095:O2136 O2332:O65044 O9:O10 O12:O606 J12:J606">
+  <conditionalFormatting sqref="J623:J747 J749 J751 J753 J755 J757 J759 J761 J763 J765:J771 J919:J1042 J1044:J1181 J1186:J1200 J1205:J1209 J1214:J1263 J1267:J1291 J1293:J1385 J1389:J1413 J1415:J1474 J1476:J1562 J1601:J1622 J1759:J1760 J1763:J1790 J1918:J1959 J1962:J1964 J1967 J1969:J1971 J1974:J2011 J2014:J2054 J2057:J2079 J2082:J2085 J2088 J2090:J2092 J2095:J2136 J2332:J65044 J9:J10 O623:O747 O749 O751 O753 O755 O757 O759 O761 O763 O765:O771 O919:O1042 O1044:O1181 O1186:O1200 O1205:O1209 O1214:O1263 O1267:O1291 O1293:O1385 O1389:O1413 O1415:O1474 O1476:O1562 O1601:O1622 O1759:O1760 O1763:O1790 O1918:O1959 O1962:O1964 O1967 O1969:O1971 O1974:O2011 O2014:O2054 O2057:O2079 O2082:O2085 O2088 O2090:O2092 O2095:O2136 O2332:O65044 O9:O10 J12:J15 J88:J606 O60:O73 O12:O15 O88:O606">
     <cfRule type="cellIs" dxfId="46" priority="68" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -6299,170 +6995,145 @@
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12:I73 N12:N73">
-    <cfRule type="cellIs" dxfId="43" priority="60" operator="equal">
+  <conditionalFormatting sqref="I12:I15 I38 I60 N60:N73 N38 N12:N15">
+    <cfRule type="cellIs" dxfId="6" priority="60" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="61" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="62" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="63" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="64" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12:I73 N12:N73">
-    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
+  <conditionalFormatting sqref="I12:I15 I38 I60 N60:N73 N38 N12:N15">
+    <cfRule type="cellIs" dxfId="1" priority="45" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="46" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T623:T747 T749 T751 T753 T755 T757 T759 T761 T763 T765:T771 T919:T1042 T1044:T1181 T1186:T1200 T1205:T1209 T1214:T1263 T1267:T1291 T1293:T1385 T1389:T1413 T1415:T1474 T1476:T1562 T1601:T1622 T1759:T1760 T1763:T1790 T1918:T1959 T1962:T1964 T1967 T1969:T1971 T1974:T2011 T2014:T2054 T2057:T2079 T2082:T2085 T2088 T2090:T2092 T2095:T2136 T2332:T65044 T9:T10 T12:T606">
-    <cfRule type="cellIs" dxfId="36" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="35" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="36" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="37" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12:S73">
-    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="31" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="32" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="33" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12:S73">
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="28" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="29" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="cellIs" dxfId="26" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="26" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="27" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="23" priority="20" operator="equal">
-      <formula>"To Be Completed"</formula>
+  <conditionalFormatting sqref="S11">
+    <cfRule type="cellIs" dxfId="23" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="24" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
-      <formula>"Fallo"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
-    <cfRule type="cellIs" dxfId="16" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" stopIfTrue="1" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P67:P68 K67:K68 U67:U68"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I73 S12:S73 N12:N73 M11 R11">
+    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P67:P68 U67:U68" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I60 S12:S73 R11 I11:I15 I38 N60:N73 N12:N15 N38" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Pendiente de Ejecución,Paso,Fallo,Bloqueado,No aplica"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B11:B15 B38 B60">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B11:B15 B38 B60 B74" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6473,11 +7144,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6535,113 +7206,231 @@
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
         <v>1</v>
       </c>
       <c r="B4" s="17"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="36">
+        <v>44859.576388888891</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="17">
+        <v>4</v>
+      </c>
+      <c r="C5" s="119">
+        <v>44859.586111111108</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
         <v>3</v>
       </c>
       <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C6" s="119">
+        <v>44859.59652777778</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
         <v>4</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="17">
+        <v>6</v>
+      </c>
+      <c r="C7" s="119">
+        <v>44859.599305555559</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
         <v>5</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="17">
+        <v>8</v>
+      </c>
+      <c r="C8" s="119">
+        <v>44859.600694444445</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
         <v>6</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="17">
+        <v>6</v>
+      </c>
+      <c r="C9" s="119">
+        <v>44859.607638888891</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>7</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="17">
+        <v>7</v>
+      </c>
+      <c r="C10" s="119">
+        <v>44859.611111111109</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
         <v>8</v>
       </c>
       <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="119">
+        <v>44859.618055555555</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <v>9</v>
       </c>
       <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
+      <c r="C12" s="119">
+        <v>44859.634722222225</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="16">
@@ -6717,17 +7506,18 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Bloqueante,Critico,Severo,Menor,Cosmetico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Creado,En Desarrollo,En Prueba,Resuelto,Bloqueado,Cancelado,Cerrado"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>